<commit_message>
Finalize first draft of crosswalk, ready for implementation
</commit_message>
<xml_diff>
--- a/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
+++ b/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\GMacDonald\Documents\ipums-acs-naics-standardization\data\manual-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D643F096-DE82-483F-81D5-3E9A278FE7BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB63E95E-1F68-49DD-B391-D6F1F13B3CE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="9600" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="9600" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017 Census Industry Code List" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="545">
   <si>
     <t>2017 Industry Code List</t>
   </si>
@@ -1543,6 +1543,141 @@
   </si>
   <si>
     <t>43000000+44220000</t>
+  </si>
+  <si>
+    <t>43485400+43485500+43485900</t>
+  </si>
+  <si>
+    <t>Made a decision to recode as US Postal Service</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>Made decision to treat as 2213</t>
+  </si>
+  <si>
+    <t>50511100-50511110</t>
+  </si>
+  <si>
+    <t>Made decision to combine as 512</t>
+  </si>
+  <si>
+    <t>50517000-50517311</t>
+  </si>
+  <si>
+    <t>Made a decision to treat as 518</t>
+  </si>
+  <si>
+    <t>Made a decision to treat as 519</t>
+  </si>
+  <si>
+    <t>55520000+55530000</t>
+  </si>
+  <si>
+    <t>55521000+55522110+55522120+55522190</t>
+  </si>
+  <si>
+    <t>Made a decision to combine 521,52211,52219,52212, and 52213</t>
+  </si>
+  <si>
+    <t>55522200+55522300</t>
+  </si>
+  <si>
+    <t>55531100+55531200</t>
+  </si>
+  <si>
+    <t>55532200+55532300</t>
+  </si>
+  <si>
+    <t>Made a decision to combine as 5322, 5323</t>
+  </si>
+  <si>
+    <t>55532400+55533000</t>
+  </si>
+  <si>
+    <t>60540000+60550000+60560000</t>
+  </si>
+  <si>
+    <t>60541900-60541940</t>
+  </si>
+  <si>
+    <t>60561700-60561730</t>
+  </si>
+  <si>
+    <t>60561100+60561200+60561900</t>
+  </si>
+  <si>
+    <t>65610000+65620000</t>
+  </si>
+  <si>
+    <t>65611200+65611300</t>
+  </si>
+  <si>
+    <t>65611400+65611500</t>
+  </si>
+  <si>
+    <t>65611600+65611700</t>
+  </si>
+  <si>
+    <t>65621300-65621310-65621320</t>
+  </si>
+  <si>
+    <t>65621500+65621900</t>
+  </si>
+  <si>
+    <t>65622100+65622300</t>
+  </si>
+  <si>
+    <t>70710000+70720000</t>
+  </si>
+  <si>
+    <t>70713000-70713950</t>
+  </si>
+  <si>
+    <t>70721200+70721199</t>
+  </si>
+  <si>
+    <t>70722000-70722400</t>
+  </si>
+  <si>
+    <t>Made decision to include 721310 and 721199 in addition to 7212, note this may cause a little overlap</t>
+  </si>
+  <si>
+    <t>80811100-80811192</t>
+  </si>
+  <si>
+    <t>Made a decision to combine 812111 and 812112</t>
+  </si>
+  <si>
+    <t>80812113+80812190</t>
+  </si>
+  <si>
+    <t>80813200+80813300+80813400</t>
+  </si>
+  <si>
+    <t>80813900-80813930</t>
+  </si>
+  <si>
+    <t>80813000-80813200-80813300-80813400-80813900</t>
+  </si>
+  <si>
+    <t>Made a decision to calculate it as the residual of 813</t>
+  </si>
+  <si>
+    <t>R81</t>
+  </si>
+  <si>
+    <t>Made a decision to calculate as the residual of 81</t>
+  </si>
+  <si>
+    <t>Made a decision to code as general government, no subcodes available, minus military and postal service</t>
+  </si>
+  <si>
+    <t>90000000-90919110-90919120</t>
+  </si>
+  <si>
+    <t>Made a decision to code as department of defense</t>
   </si>
 </sst>
 </file>
@@ -2013,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C169" workbookViewId="0">
-      <selection activeCell="F183" sqref="F183"/>
+    <sheetView tabSelected="1" topLeftCell="C337" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4876,7 +5011,7 @@
         <v>232</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>444</v>
+        <v>500</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
@@ -4950,8 +5085,11 @@
       <c r="E188" s="5">
         <v>491</v>
       </c>
-      <c r="F188" s="1" t="s">
-        <v>444</v>
+      <c r="F188" s="1">
+        <v>90919120</v>
+      </c>
+      <c r="G188" s="33" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
@@ -5063,7 +5201,7 @@
         <v>248</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="G196" s="33"/>
       <c r="I196" s="7"/>
@@ -5082,10 +5220,12 @@
       <c r="E197" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F197" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G197" s="33"/>
+      <c r="F197" s="1">
+        <v>44221300</v>
+      </c>
+      <c r="G197" s="33" t="s">
+        <v>503</v>
+      </c>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
       <c r="K197" s="7"/>
@@ -5102,10 +5242,12 @@
       <c r="E198" s="5">
         <v>22132</v>
       </c>
-      <c r="F198" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G198" s="33"/>
+      <c r="F198" s="1">
+        <v>44221300</v>
+      </c>
+      <c r="G198" s="33" t="s">
+        <v>503</v>
+      </c>
       <c r="I198" s="7"/>
       <c r="J198" s="7"/>
       <c r="K198" s="7"/>
@@ -5123,7 +5265,7 @@
         <v>256</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>444</v>
+        <v>502</v>
       </c>
       <c r="G199" s="33"/>
       <c r="I199" s="7"/>
@@ -5200,7 +5342,7 @@
         <v>261</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>444</v>
+        <v>504</v>
       </c>
       <c r="G204" s="33"/>
       <c r="I204" s="7"/>
@@ -5239,10 +5381,12 @@
       <c r="E206" s="5">
         <v>5121</v>
       </c>
-      <c r="F206" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G206" s="33"/>
+      <c r="F206" s="1">
+        <v>50512000</v>
+      </c>
+      <c r="G206" s="33" t="s">
+        <v>505</v>
+      </c>
       <c r="I206" s="7"/>
       <c r="J206" s="7"/>
       <c r="K206" s="7"/>
@@ -5259,10 +5403,12 @@
       <c r="E207" s="5">
         <v>5122</v>
       </c>
-      <c r="F207" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G207" s="33"/>
+      <c r="F207" s="1">
+        <v>50512000</v>
+      </c>
+      <c r="G207" s="33" t="s">
+        <v>505</v>
+      </c>
       <c r="I207" s="7"/>
       <c r="J207" s="7"/>
       <c r="K207" s="7"/>
@@ -5340,7 +5486,7 @@
         <v>431</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>444</v>
+        <v>506</v>
       </c>
       <c r="I211" s="1"/>
       <c r="J211" s="1"/>
@@ -5357,10 +5503,12 @@
       <c r="E212" s="5">
         <v>5182</v>
       </c>
-      <c r="F212" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G212" s="33"/>
+      <c r="F212" s="1">
+        <v>50518000</v>
+      </c>
+      <c r="G212" s="33" t="s">
+        <v>507</v>
+      </c>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
       <c r="K212" s="7"/>
@@ -5377,10 +5525,12 @@
       <c r="E213" s="5">
         <v>51912</v>
       </c>
-      <c r="F213" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G213" s="33"/>
+      <c r="F213" s="1">
+        <v>50519000</v>
+      </c>
+      <c r="G213" s="33" t="s">
+        <v>508</v>
+      </c>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
       <c r="K213" s="7"/>
@@ -5397,10 +5547,12 @@
       <c r="E214" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="F214" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G214" s="33"/>
+      <c r="F214" s="1">
+        <v>50519000</v>
+      </c>
+      <c r="G214" s="33" t="s">
+        <v>508</v>
+      </c>
       <c r="I214" s="7"/>
       <c r="J214" s="7"/>
       <c r="K214" s="7"/>
@@ -5431,7 +5583,7 @@
         <v>275</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>444</v>
+        <v>509</v>
       </c>
       <c r="G216" s="33"/>
       <c r="I216" s="7"/>
@@ -5497,14 +5649,16 @@
         <v>279</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G220" s="33"/>
+        <v>510</v>
+      </c>
+      <c r="G220" s="33" t="s">
+        <v>511</v>
+      </c>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
       <c r="K220" s="7"/>
     </row>
-    <row r="221" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A221" s="3"/>
       <c r="B221" s="1" t="s">
         <v>280</v>
@@ -5517,9 +5671,11 @@
         <v>281</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="G221" s="33"/>
+        <v>510</v>
+      </c>
+      <c r="G221" s="33" t="s">
+        <v>511</v>
+      </c>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
       <c r="K221" s="7"/>
@@ -5536,7 +5692,7 @@
         <v>283</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>444</v>
+        <v>512</v>
       </c>
     </row>
     <row r="223" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5550,8 +5706,8 @@
       <c r="E223" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="F223" s="1" t="s">
-        <v>444</v>
+      <c r="F223" s="1">
+        <v>55523000</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
@@ -5568,7 +5724,7 @@
         <v>55524100</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B225" s="1" t="s">
         <v>287</v>
       </c>
@@ -5582,12 +5738,12 @@
         <v>55524200</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F226" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B227" s="30" t="s">
         <v>288</v>
       </c>
@@ -5601,13 +5757,13 @@
         <v>55530000</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
       <c r="F228" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="3"/>
       <c r="B229" s="1" t="s">
         <v>290</v>
@@ -5619,10 +5775,10 @@
         <v>291</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="3"/>
       <c r="B230" s="1" t="s">
         <v>292</v>
@@ -5637,14 +5793,14 @@
         <v>55531300</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="3"/>
       <c r="D231" s="3"/>
       <c r="F231" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="3"/>
       <c r="B232" s="1" t="s">
         <v>293</v>
@@ -5659,7 +5815,7 @@
         <v>55532100</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="6"/>
       <c r="B233" s="1" t="s">
         <v>294</v>
@@ -5671,10 +5827,13 @@
         <v>295</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="G233" s="33" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B234" s="1" t="s">
         <v>296</v>
       </c>
@@ -5685,15 +5844,15 @@
         <v>297</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F235" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="8" t="s">
         <v>298</v>
       </c>
@@ -5706,10 +5865,10 @@
         <v>300</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="8" t="s">
         <v>301</v>
       </c>
@@ -5721,13 +5880,13 @@
         <v>444</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D238" s="3"/>
       <c r="F238" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B239" s="30" t="s">
         <v>302</v>
       </c>
@@ -5741,7 +5900,7 @@
         <v>60540000</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="F240" s="1" t="s">
         <v>444</v>
@@ -5920,7 +6079,7 @@
         <v>314</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>444</v>
+        <v>518</v>
       </c>
       <c r="G250" s="33"/>
       <c r="I250" s="7"/>
@@ -6098,7 +6257,7 @@
         <v>324</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>444</v>
+        <v>519</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
@@ -6128,7 +6287,7 @@
         <v>327</v>
       </c>
       <c r="F264" s="1" t="s">
-        <v>444</v>
+        <v>520</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
@@ -6162,7 +6321,7 @@
         <v>331</v>
       </c>
       <c r="F267" s="1" t="s">
-        <v>444</v>
+        <v>521</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
@@ -6219,7 +6378,7 @@
         <v>336</v>
       </c>
       <c r="F272" s="1" t="s">
-        <v>444</v>
+        <v>522</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
@@ -6234,7 +6393,7 @@
         <v>338</v>
       </c>
       <c r="F273" s="1" t="s">
-        <v>444</v>
+        <v>523</v>
       </c>
     </row>
     <row r="274" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6248,7 +6407,7 @@
         <v>340</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>444</v>
+        <v>524</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
@@ -6350,7 +6509,7 @@
         <v>348</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>444</v>
+        <v>525</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -6395,7 +6554,7 @@
         <v>352</v>
       </c>
       <c r="F285" s="1" t="s">
-        <v>444</v>
+        <v>526</v>
       </c>
     </row>
     <row r="286" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6410,7 +6569,7 @@
         <v>353</v>
       </c>
       <c r="F286" s="1" t="s">
-        <v>444</v>
+        <v>527</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
@@ -6534,7 +6693,7 @@
         <v>364</v>
       </c>
       <c r="F295" s="1" t="s">
-        <v>444</v>
+        <v>528</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
@@ -6605,8 +6764,8 @@
       <c r="E301" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="F301" s="1" t="s">
-        <v>444</v>
+      <c r="F301" s="1">
+        <v>70711300</v>
       </c>
     </row>
     <row r="302" spans="1:6" x14ac:dyDescent="0.25">
@@ -6654,7 +6813,7 @@
         <v>70713950</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B305" s="1" t="s">
         <v>374</v>
       </c>
@@ -6665,15 +6824,15 @@
         <v>375</v>
       </c>
       <c r="F305" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F306" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B307" s="30" t="s">
         <v>376</v>
       </c>
@@ -6688,13 +6847,13 @@
         <v>70720000</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="3"/>
       <c r="F308" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="6"/>
       <c r="B309" s="1" t="s">
         <v>378</v>
@@ -6709,7 +6868,7 @@
         <v>70721100</v>
       </c>
     </row>
-    <row r="310" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="3"/>
       <c r="B310" s="1" t="s">
         <v>379</v>
@@ -6721,10 +6880,13 @@
         <v>380</v>
       </c>
       <c r="F310" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="G310" s="33" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311" s="3"/>
       <c r="B311" s="1" t="s">
         <v>381</v>
@@ -6736,10 +6898,10 @@
         <v>382</v>
       </c>
       <c r="F311" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B312" s="1" t="s">
         <v>383</v>
       </c>
@@ -6753,12 +6915,12 @@
         <v>70722400</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F313" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A314" s="8" t="s">
         <v>384</v>
       </c>
@@ -6773,13 +6935,13 @@
         <v>80000000</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="3"/>
       <c r="F315" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="316" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A316" s="3"/>
       <c r="B316" s="1" t="s">
         <v>386</v>
@@ -6791,10 +6953,10 @@
         <v>387</v>
       </c>
       <c r="F316" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A317" s="6"/>
       <c r="B317" s="1" t="s">
         <v>388</v>
@@ -6809,7 +6971,7 @@
         <v>80811192</v>
       </c>
     </row>
-    <row r="318" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A318" s="6"/>
       <c r="B318" s="1" t="s">
         <v>389</v>
@@ -6824,7 +6986,7 @@
         <v>80811200</v>
       </c>
     </row>
-    <row r="319" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A319" s="3"/>
       <c r="B319" s="1" t="s">
         <v>390</v>
@@ -6839,7 +7001,7 @@
         <v>80811300</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A320" s="3"/>
       <c r="B320" s="1" t="s">
         <v>391</v>
@@ -6854,7 +7016,7 @@
         <v>80811400</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A321" s="3"/>
       <c r="B321" s="1" t="s">
         <v>392</v>
@@ -6865,11 +7027,14 @@
       <c r="E321" s="5">
         <v>812111</v>
       </c>
-      <c r="F321" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F321" s="1">
+        <v>80812112</v>
+      </c>
+      <c r="G321" s="33" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A322" s="3"/>
       <c r="B322" s="1" t="s">
         <v>393</v>
@@ -6880,11 +7045,14 @@
       <c r="E322" s="5">
         <v>812112</v>
       </c>
-      <c r="F322" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F322" s="1">
+        <v>80812112</v>
+      </c>
+      <c r="G322" s="33" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A323" s="3"/>
       <c r="B323" s="1" t="s">
         <v>394</v>
@@ -6896,10 +7064,10 @@
         <v>395</v>
       </c>
       <c r="F323" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A324" s="3"/>
       <c r="B324" s="1" t="s">
         <v>396</v>
@@ -6914,7 +7082,7 @@
         <v>80812300</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A325" s="3"/>
       <c r="B325" s="1" t="s">
         <v>397</v>
@@ -6929,7 +7097,7 @@
         <v>80812200</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A326" s="3"/>
       <c r="B326" s="1" t="s">
         <v>398</v>
@@ -6944,7 +7112,7 @@
         <v>80812900</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A327" s="6"/>
       <c r="B327" s="1" t="s">
         <v>399</v>
@@ -6956,10 +7124,13 @@
         <v>8131</v>
       </c>
       <c r="F327" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="328" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+      <c r="G327" s="33" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A328" s="3"/>
       <c r="B328" s="1" t="s">
         <v>400</v>
@@ -6971,10 +7142,10 @@
         <v>401</v>
       </c>
       <c r="F328" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A329" s="6"/>
       <c r="B329" s="1" t="s">
         <v>402</v>
@@ -6989,7 +7160,7 @@
         <v>80813930</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A330" s="3"/>
       <c r="B330" s="1" t="s">
         <v>403</v>
@@ -7001,10 +7172,10 @@
         <v>404</v>
       </c>
       <c r="F330" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B331" s="1" t="s">
         <v>405</v>
       </c>
@@ -7015,15 +7186,18 @@
         <v>814</v>
       </c>
       <c r="F331" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+      <c r="G331" s="33" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F332" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A333" s="8" t="s">
         <v>406</v>
       </c>
@@ -7034,16 +7208,19 @@
         <v>92</v>
       </c>
       <c r="F333" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G333" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" s="3"/>
       <c r="F334" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="335" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A335" s="3"/>
       <c r="B335" s="1" t="s">
         <v>408</v>
@@ -7055,10 +7232,13 @@
         <v>409</v>
       </c>
       <c r="F335" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G335" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A336" s="3"/>
       <c r="B336" s="1" t="s">
         <v>410</v>
@@ -7070,10 +7250,13 @@
         <v>92113</v>
       </c>
       <c r="F336" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G336" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A337" s="3"/>
       <c r="B337" s="1" t="s">
         <v>411</v>
@@ -7085,10 +7268,13 @@
         <v>92119</v>
       </c>
       <c r="F337" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G337" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A338" s="3"/>
       <c r="B338" s="1" t="s">
         <v>412</v>
@@ -7100,10 +7286,13 @@
         <v>413</v>
       </c>
       <c r="F338" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G338" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A339" s="6"/>
       <c r="B339" s="1" t="s">
         <v>414</v>
@@ -7115,10 +7304,13 @@
         <v>923</v>
       </c>
       <c r="F339" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="340" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G339" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A340" s="6"/>
       <c r="B340" s="1" t="s">
         <v>415</v>
@@ -7130,10 +7322,13 @@
         <v>416</v>
       </c>
       <c r="F340" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G340" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A341" s="3"/>
       <c r="B341" s="1" t="s">
         <v>417</v>
@@ -7145,10 +7340,13 @@
         <v>418</v>
       </c>
       <c r="F341" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G341" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B342" s="1" t="s">
         <v>419</v>
       </c>
@@ -7159,15 +7357,18 @@
         <v>928</v>
       </c>
       <c r="F342" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+      <c r="G342" s="33" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F343" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A344" s="8" t="s">
         <v>420</v>
       </c>
@@ -7177,18 +7378,21 @@
       <c r="E344" s="5">
         <v>928110</v>
       </c>
-      <c r="F344" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F344" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G344" s="33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B345" s="20"/>
       <c r="D345" s="3"/>
       <c r="F345" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A346" s="3"/>
       <c r="B346" s="1" t="s">
         <v>422</v>
@@ -7199,11 +7403,14 @@
       <c r="E346" s="5">
         <v>928110</v>
       </c>
-      <c r="F346" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F346" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G346" s="33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A347" s="3"/>
       <c r="B347" s="1" t="s">
         <v>423</v>
@@ -7214,11 +7421,14 @@
       <c r="E347" s="5">
         <v>928110</v>
       </c>
-      <c r="F347" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F347" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G347" s="33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A348" s="3"/>
       <c r="B348" s="1" t="s">
         <v>424</v>
@@ -7229,11 +7439,14 @@
       <c r="E348" s="5">
         <v>928110</v>
       </c>
-      <c r="F348" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F348" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G348" s="33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A349" s="3"/>
       <c r="B349" s="1" t="s">
         <v>425</v>
@@ -7244,11 +7457,14 @@
       <c r="E349" s="5">
         <v>928110</v>
       </c>
-      <c r="F349" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F349" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G349" s="33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B350" s="1" t="s">
         <v>426</v>
       </c>
@@ -7258,11 +7474,14 @@
       <c r="E350" s="5">
         <v>928110</v>
       </c>
-      <c r="F350" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F350" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G350" s="33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B351" s="1" t="s">
         <v>427</v>
       </c>
@@ -7272,11 +7491,14 @@
       <c r="E351" s="5">
         <v>928110</v>
       </c>
-      <c r="F351" s="1" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F351" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G351" s="33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B352" s="1" t="s">
         <v>428</v>
       </c>
@@ -7286,8 +7508,11 @@
       <c r="E352" s="5">
         <v>928110</v>
       </c>
-      <c r="F352" s="1" t="s">
-        <v>444</v>
+      <c r="F352" s="1">
+        <v>90919110</v>
+      </c>
+      <c r="G352" s="33" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="353" spans="2:6" x14ac:dyDescent="0.25">
@@ -7304,7 +7529,7 @@
         <v>9920</v>
       </c>
       <c r="F354" s="1" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="355" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create residual rules, finalize clean crosswalk
</commit_message>
<xml_diff>
--- a/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
+++ b/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\GMacDonald\Documents\ipums-acs-naics-standardization\data\manual-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB63E95E-1F68-49DD-B391-D6F1F13B3CE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C1ACF4-D228-4A71-9F88-63CFE90CF334}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="9600" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15435" yWindow="45" windowWidth="9600" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017 Census Industry Code List" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="542">
   <si>
     <t>2017 Industry Code List</t>
   </si>
@@ -1359,9 +1359,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Residual is mostly 11 agrigultural which BLS doesn't have</t>
-  </si>
-  <si>
     <t>32311100+32311200</t>
   </si>
   <si>
@@ -1371,12 +1368,6 @@
     <t>32311700+32311900</t>
   </si>
   <si>
-    <t>Residual of 311</t>
-  </si>
-  <si>
-    <t>Residual of 21, will want to investigate how to deal with these</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -1422,36 +1413,9 @@
     <t>31332600+31332900-31332994</t>
   </si>
   <si>
-    <t>Residual of 331 and 332</t>
-  </si>
-  <si>
     <t>31333120+31333130</t>
   </si>
   <si>
-    <t>10113300+10210000+R11</t>
-  </si>
-  <si>
-    <t>R331+R332</t>
-  </si>
-  <si>
-    <t>R311</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>Made decision to combine as residual of 31</t>
-  </si>
-  <si>
-    <t>31333200+31333400+31333900+R333</t>
-  </si>
-  <si>
-    <t>Note residual of 333</t>
-  </si>
-  <si>
     <t>31334200+31334400+31334600</t>
   </si>
   <si>
@@ -1488,12 +1452,6 @@
     <t>Made decision to only exclude 33992</t>
   </si>
   <si>
-    <t>R31+R32+R33</t>
-  </si>
-  <si>
-    <t>Residual of manufacturing in general</t>
-  </si>
-  <si>
     <t>41423900-41423930</t>
   </si>
   <si>
@@ -1509,9 +1467,6 @@
     <t>Made decision to treat as 42511+42512</t>
   </si>
   <si>
-    <t>R42</t>
-  </si>
-  <si>
     <t>42444100-42444130</t>
   </si>
   <si>
@@ -1536,12 +1491,6 @@
     <t>Made decision to treat as 45431</t>
   </si>
   <si>
-    <t>R44+R45</t>
-  </si>
-  <si>
-    <t>Residual of retail trade in general</t>
-  </si>
-  <si>
     <t>43000000+44220000</t>
   </si>
   <si>
@@ -1551,9 +1500,6 @@
     <t>Made a decision to recode as US Postal Service</t>
   </si>
   <si>
-    <t>R22</t>
-  </si>
-  <si>
     <t>Made decision to treat as 2213</t>
   </si>
   <si>
@@ -1665,9 +1611,6 @@
     <t>Made a decision to calculate it as the residual of 813</t>
   </si>
   <si>
-    <t>R81</t>
-  </si>
-  <si>
     <t>Made a decision to calculate as the residual of 81</t>
   </si>
   <si>
@@ -1678,6 +1621,54 @@
   </si>
   <si>
     <t>Made a decision to code as department of defense</t>
+  </si>
+  <si>
+    <t>65623200+65623300+65623900</t>
+  </si>
+  <si>
+    <t>10113300+10210000</t>
+  </si>
+  <si>
+    <t>Residual is mostly 11 agrigultural which BLS doesn't have, so left out here</t>
+  </si>
+  <si>
+    <t>10210000-10211000-10212100-10212200-10212300-10213000</t>
+  </si>
+  <si>
+    <t>Made decision to treat residuals as category minus everything else defined</t>
+  </si>
+  <si>
+    <t>32311000-32311100-32311200-32311300-32311400-32311500-32311600-32311800-32311700-32311900</t>
+  </si>
+  <si>
+    <t>31331000+31332000-31331100-31331200-31331300-31331400-31331500-31332100-31332200-31332300-31332400-31332700-31332800-31332994-31332600-31332900</t>
+  </si>
+  <si>
+    <t>Made decision to treat as residual of 333, residuals as category minus everything else defined</t>
+  </si>
+  <si>
+    <t>31333000-31333110-31333120-31333130-31333300-31333500-31333600</t>
+  </si>
+  <si>
+    <t>Made decision to combine as residual of 31, 32, and 33, because there is no 31 in BLS data so impossible to estimate</t>
+  </si>
+  <si>
+    <t>30000000-31321000-31327000-31331000-31332000-31333000-31334000-31335000-31336000-31337000-31339000-32311000-32313000-32314000-32315000-32322000-32323000-32324000-32325000-32326000-32329100-32329900</t>
+  </si>
+  <si>
+    <t>41420000-41423000-41424000-41425110-41425120</t>
+  </si>
+  <si>
+    <t>42000000-42441000-42442000-42443000-42444000-42445000-42446000-42447000-42448000-42451000-42452000-42453000-42454000</t>
+  </si>
+  <si>
+    <t>Made decision to treat residuals as category minus everything else defined, could be 0, given other definitions and decisions made here</t>
+  </si>
+  <si>
+    <t>44220000-44221100-44221200-44221300</t>
+  </si>
+  <si>
+    <t>80000000-80811000-80812000-80813000</t>
   </si>
 </sst>
 </file>
@@ -2148,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C337" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,10 +2217,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>461</v>
+        <v>527</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>438</v>
+        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2419,7 +2410,7 @@
         <v>10212300</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
@@ -2431,10 +2422,10 @@
         <v>34</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>464</v>
+        <v>529</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>443</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2508,7 +2499,7 @@
         <v>44</v>
       </c>
       <c r="F33" s="37" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2599,7 +2590,7 @@
         <v>51</v>
       </c>
       <c r="F39" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2614,10 +2605,10 @@
         <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="1" t="s">
         <v>54</v>
@@ -2629,10 +2620,10 @@
         <v>55</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>463</v>
+        <v>531</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>442</v>
+        <v>530</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2665,7 +2656,7 @@
         <v>32329900</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2683,7 +2674,7 @@
         <v>32313000</v>
       </c>
       <c r="G44" s="33" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2701,7 +2692,7 @@
         <v>32313000</v>
       </c>
       <c r="G45" s="33" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,7 +2710,7 @@
         <v>32313000</v>
       </c>
       <c r="G46" s="33" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2737,7 +2728,7 @@
         <v>32314000</v>
       </c>
       <c r="G47" s="33" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2755,7 +2746,7 @@
         <v>32314000</v>
       </c>
       <c r="G48" s="33" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2773,7 +2764,7 @@
         <v>32315000</v>
       </c>
       <c r="G49" s="33" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2791,10 +2782,10 @@
         <v>32315000</v>
       </c>
       <c r="G50" s="33" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
         <v>69</v>
@@ -2805,14 +2796,14 @@
       <c r="E51" s="12">
         <v>3162</v>
       </c>
-      <c r="F51" t="s">
-        <v>465</v>
+      <c r="F51" s="1" t="s">
+        <v>536</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="1" t="s">
         <v>70</v>
@@ -2823,11 +2814,11 @@
       <c r="E52" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F52" t="s">
-        <v>465</v>
+      <c r="F52" s="1" t="s">
+        <v>536</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>466</v>
+        <v>535</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2872,7 +2863,7 @@
         <v>75</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2890,7 +2881,7 @@
         <v>32323000</v>
       </c>
       <c r="G56" s="33" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3010,7 +3001,7 @@
         <v>86</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -3073,7 +3064,7 @@
         <v>31327100</v>
       </c>
       <c r="G68" s="33" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -3091,7 +3082,7 @@
         <v>31327100</v>
       </c>
       <c r="G69" s="33" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3120,10 +3111,10 @@
         <v>95</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G71" s="33" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3138,10 +3129,10 @@
         <v>3279</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G72" s="33" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -3156,7 +3147,7 @@
         <v>98</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -3252,7 +3243,7 @@
         <v>105</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G79" s="33"/>
       <c r="I79" s="7"/>
@@ -3315,7 +3306,7 @@
         <v>31332994</v>
       </c>
       <c r="G82" s="33" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
@@ -3334,16 +3325,16 @@
         <v>111</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="G83" s="33" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
     </row>
-    <row r="84" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="1" t="s">
         <v>112</v>
@@ -3356,10 +3347,10 @@
         <v>113</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>462</v>
+        <v>532</v>
       </c>
       <c r="G84" s="33" t="s">
-        <v>459</v>
+        <v>530</v>
       </c>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
@@ -3398,7 +3389,7 @@
         <v>116</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="G86" s="33"/>
       <c r="I86" s="7"/>
@@ -3478,10 +3469,10 @@
         <v>121</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>467</v>
+        <v>534</v>
       </c>
       <c r="G90" s="33" t="s">
-        <v>468</v>
+        <v>533</v>
       </c>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
@@ -3520,10 +3511,10 @@
         <v>124</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="G92" s="33" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
@@ -3562,10 +3553,10 @@
         <v>127</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="G94" s="33" t="s">
-        <v>470</v>
+        <v>458</v>
       </c>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
@@ -3603,7 +3594,7 @@
         <v>130</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="G96" s="33"/>
       <c r="I96" s="7"/>
@@ -3623,7 +3614,7 @@
         <v>132</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="G97" s="33"/>
       <c r="I97" s="7"/>
@@ -3643,7 +3634,7 @@
         <v>134</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>473</v>
+        <v>461</v>
       </c>
       <c r="G98" s="33"/>
       <c r="I98" s="7"/>
@@ -3686,7 +3677,7 @@
         <v>31336900</v>
       </c>
       <c r="G100" s="33" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
@@ -3728,7 +3719,7 @@
         <v>31336900</v>
       </c>
       <c r="G102" s="33" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
@@ -3790,7 +3781,7 @@
         <v>31321990</v>
       </c>
       <c r="G105" s="33" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
@@ -3809,10 +3800,10 @@
         <v>144</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="G106" s="33" t="s">
-        <v>477</v>
+        <v>465</v>
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
@@ -3863,7 +3854,7 @@
         <v>31339920</v>
       </c>
       <c r="G109" s="33" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
     </row>
     <row r="110" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3878,13 +3869,13 @@
         <v>150</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="G110" s="33" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="1" t="s">
         <v>151</v>
@@ -3896,17 +3887,14 @@
         <v>152</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>481</v>
+        <v>536</v>
       </c>
       <c r="G111" s="33" t="s">
-        <v>482</v>
+        <v>530</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D112" s="3"/>
-      <c r="F112" s="1" t="s">
-        <v>444</v>
-      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
@@ -3925,7 +3913,7 @@
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="F114" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4085,7 +4073,7 @@
         <v>165</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -4117,7 +4105,7 @@
         <v>168</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -4229,7 +4217,7 @@
         <v>176</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4245,13 +4233,13 @@
         <v>4251</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="G134" s="33" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
         <v>178</v>
       </c>
@@ -4263,12 +4251,15 @@
         <v>179</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>488</v>
+        <v>537</v>
+      </c>
+      <c r="G135" s="33" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F136" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4288,7 +4279,7 @@
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="F138" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -4393,7 +4384,7 @@
         <v>190</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>489</v>
+        <v>474</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -4513,7 +4504,7 @@
         <v>198</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>490</v>
+        <v>475</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -4561,7 +4552,7 @@
         <v>42448200</v>
       </c>
       <c r="G156" s="33" t="s">
-        <v>491</v>
+        <v>476</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4591,7 +4582,7 @@
         <v>204</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>494</v>
+        <v>479</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -4639,7 +4630,7 @@
         <v>42451200</v>
       </c>
       <c r="G161" s="33" t="s">
-        <v>492</v>
+        <v>477</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
@@ -4657,7 +4648,7 @@
         <v>42452200</v>
       </c>
       <c r="G162" s="33" t="s">
-        <v>493</v>
+        <v>478</v>
       </c>
     </row>
     <row r="163" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4786,7 +4777,7 @@
         <v>42454100</v>
       </c>
       <c r="G169" s="33" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
@@ -4828,7 +4819,7 @@
         <v>42454310</v>
       </c>
       <c r="G171" s="33" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="I171" s="7"/>
       <c r="J171" s="7"/>
@@ -4854,7 +4845,7 @@
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
     </row>
-    <row r="173" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="1" t="s">
         <v>219</v>
@@ -4867,10 +4858,10 @@
         <v>220</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>497</v>
+        <v>538</v>
       </c>
       <c r="G173" s="33" t="s">
-        <v>498</v>
+        <v>539</v>
       </c>
       <c r="I173" s="7"/>
       <c r="J173" s="7"/>
@@ -4878,7 +4869,7 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F174" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="175" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4893,7 +4884,7 @@
         <v>223</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
       <c r="G175" s="33"/>
       <c r="I175" s="7"/>
@@ -4906,7 +4897,7 @@
       <c r="D176" s="2"/>
       <c r="E176" s="5"/>
       <c r="F176" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G176" s="33"/>
       <c r="I176" s="7"/>
@@ -4936,7 +4927,7 @@
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="F178" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
@@ -5011,7 +5002,7 @@
         <v>232</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
@@ -5089,7 +5080,7 @@
         <v>90919120</v>
       </c>
       <c r="G188" s="33" t="s">
-        <v>501</v>
+        <v>484</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
@@ -5125,7 +5116,7 @@
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D191" s="3"/>
       <c r="F191" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
@@ -5145,7 +5136,7 @@
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="11"/>
       <c r="F193" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="194" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5224,7 +5215,7 @@
         <v>44221300</v>
       </c>
       <c r="G197" s="33" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
@@ -5246,13 +5237,13 @@
         <v>44221300</v>
       </c>
       <c r="G198" s="33" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="I198" s="7"/>
       <c r="J198" s="7"/>
       <c r="K198" s="7"/>
     </row>
-    <row r="199" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A199" s="7"/>
       <c r="B199" s="1" t="s">
         <v>254</v>
@@ -5265,16 +5256,18 @@
         <v>256</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="G199" s="33"/>
+        <v>540</v>
+      </c>
+      <c r="G199" s="33" t="s">
+        <v>539</v>
+      </c>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
       <c r="K199" s="7"/>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F200" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="201" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5302,7 +5295,7 @@
       <c r="D202" s="7"/>
       <c r="E202" s="5"/>
       <c r="F202" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G202" s="33"/>
       <c r="I202" s="7"/>
@@ -5342,7 +5335,7 @@
         <v>261</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="G204" s="33"/>
       <c r="I204" s="7"/>
@@ -5385,7 +5378,7 @@
         <v>50512000</v>
       </c>
       <c r="G206" s="33" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="I206" s="7"/>
       <c r="J206" s="7"/>
@@ -5407,7 +5400,7 @@
         <v>50512000</v>
       </c>
       <c r="G207" s="33" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
       <c r="I207" s="7"/>
       <c r="J207" s="7"/>
@@ -5486,7 +5479,7 @@
         <v>431</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="I211" s="1"/>
       <c r="J211" s="1"/>
@@ -5507,7 +5500,7 @@
         <v>50518000</v>
       </c>
       <c r="G212" s="33" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
@@ -5529,7 +5522,7 @@
         <v>50519000</v>
       </c>
       <c r="G213" s="33" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
@@ -5551,7 +5544,7 @@
         <v>50519000</v>
       </c>
       <c r="G214" s="33" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
       <c r="I214" s="7"/>
       <c r="J214" s="7"/>
@@ -5563,7 +5556,7 @@
       <c r="D215" s="3"/>
       <c r="E215" s="5"/>
       <c r="F215" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G215" s="33"/>
       <c r="I215" s="7"/>
@@ -5583,7 +5576,7 @@
         <v>275</v>
       </c>
       <c r="F216" s="1" t="s">
-        <v>509</v>
+        <v>491</v>
       </c>
       <c r="G216" s="33"/>
       <c r="I216" s="7"/>
@@ -5596,7 +5589,7 @@
       <c r="D217" s="3"/>
       <c r="E217" s="5"/>
       <c r="F217" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G217" s="33"/>
       <c r="I217" s="7"/>
@@ -5629,7 +5622,7 @@
       <c r="D219" s="7"/>
       <c r="E219" s="5"/>
       <c r="F219" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G219" s="33"/>
       <c r="I219" s="7"/>
@@ -5649,10 +5642,10 @@
         <v>279</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="G220" s="33" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
@@ -5671,10 +5664,10 @@
         <v>281</v>
       </c>
       <c r="F221" s="1" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
       <c r="G221" s="33" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
@@ -5692,7 +5685,7 @@
         <v>283</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
     </row>
     <row r="223" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5740,7 +5733,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F226" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -5760,7 +5753,7 @@
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
       <c r="F228" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="229" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5775,7 +5768,7 @@
         <v>291</v>
       </c>
       <c r="F229" s="1" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
     </row>
     <row r="230" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5797,7 +5790,7 @@
       <c r="A231" s="3"/>
       <c r="D231" s="3"/>
       <c r="F231" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -5827,10 +5820,10 @@
         <v>295</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
       <c r="G233" s="33" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
     </row>
     <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5844,12 +5837,12 @@
         <v>297</v>
       </c>
       <c r="F234" s="1" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F235" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -5865,7 +5858,7 @@
         <v>300</v>
       </c>
       <c r="F236" s="1" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -5877,13 +5870,13 @@
       <c r="D237" s="3"/>
       <c r="E237" s="21"/>
       <c r="F237" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D238" s="3"/>
       <c r="F238" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -5903,7 +5896,7 @@
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="F240" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
@@ -6079,7 +6072,7 @@
         <v>314</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
       <c r="G250" s="33"/>
       <c r="I250" s="7"/>
@@ -6088,7 +6081,7 @@
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F251" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="252" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6117,7 +6110,7 @@
       <c r="D253" s="7"/>
       <c r="E253" s="5"/>
       <c r="F253" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G253" s="33"/>
       <c r="I253" s="7"/>
@@ -6150,7 +6143,7 @@
       <c r="D255" s="3"/>
       <c r="E255" s="5"/>
       <c r="F255" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G255" s="33"/>
       <c r="I255" s="7"/>
@@ -6181,7 +6174,7 @@
       <c r="A257" s="3"/>
       <c r="D257" s="3"/>
       <c r="F257" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.25">
@@ -6257,7 +6250,7 @@
         <v>324</v>
       </c>
       <c r="F262" s="1" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.25">
@@ -6287,7 +6280,7 @@
         <v>327</v>
       </c>
       <c r="F264" s="1" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.25">
@@ -6306,7 +6299,7 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F266" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
@@ -6321,13 +6314,13 @@
         <v>331</v>
       </c>
       <c r="F267" s="1" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D268" s="3"/>
       <c r="F268" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
@@ -6348,7 +6341,7 @@
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="3"/>
       <c r="F270" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
@@ -6378,7 +6371,7 @@
         <v>336</v>
       </c>
       <c r="F272" s="1" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
@@ -6393,7 +6386,7 @@
         <v>338</v>
       </c>
       <c r="F273" s="1" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
     </row>
     <row r="274" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6407,12 +6400,12 @@
         <v>340</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F275" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.25">
@@ -6433,7 +6426,7 @@
     <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="3"/>
       <c r="F277" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.25">
@@ -6509,7 +6502,7 @@
         <v>348</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.25">
@@ -6554,7 +6547,7 @@
         <v>352</v>
       </c>
       <c r="F285" s="1" t="s">
-        <v>526</v>
+        <v>508</v>
       </c>
     </row>
     <row r="286" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6569,7 +6562,7 @@
         <v>353</v>
       </c>
       <c r="F286" s="1" t="s">
-        <v>527</v>
+        <v>509</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.25">
@@ -6614,7 +6607,7 @@
         <v>357</v>
       </c>
       <c r="F289" s="1" t="s">
-        <v>444</v>
+        <v>526</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
@@ -6678,7 +6671,7 @@
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F294" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">
@@ -6693,13 +6686,13 @@
         <v>364</v>
       </c>
       <c r="F295" s="1" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B296" s="32"/>
       <c r="F296" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
@@ -6720,7 +6713,7 @@
     <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="6"/>
       <c r="F298" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.25">
@@ -6824,12 +6817,12 @@
         <v>375</v>
       </c>
       <c r="F305" s="1" t="s">
-        <v>529</v>
+        <v>511</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F306" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.25">
@@ -6850,7 +6843,7 @@
     <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="3"/>
       <c r="F308" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.25">
@@ -6880,10 +6873,10 @@
         <v>380</v>
       </c>
       <c r="F310" s="1" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
       <c r="G310" s="33" t="s">
-        <v>532</v>
+        <v>514</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.25">
@@ -6898,7 +6891,7 @@
         <v>382</v>
       </c>
       <c r="F311" s="1" t="s">
-        <v>531</v>
+        <v>513</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
@@ -6917,7 +6910,7 @@
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F313" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
@@ -6938,7 +6931,7 @@
     <row r="315" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A315" s="3"/>
       <c r="F315" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="316" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6953,7 +6946,7 @@
         <v>387</v>
       </c>
       <c r="F316" s="1" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.25">
@@ -7031,7 +7024,7 @@
         <v>80812112</v>
       </c>
       <c r="G321" s="33" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
@@ -7049,7 +7042,7 @@
         <v>80812112</v>
       </c>
       <c r="G322" s="33" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.25">
@@ -7064,7 +7057,7 @@
         <v>395</v>
       </c>
       <c r="F323" s="1" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.25">
@@ -7124,10 +7117,10 @@
         <v>8131</v>
       </c>
       <c r="F327" s="1" t="s">
-        <v>538</v>
+        <v>520</v>
       </c>
       <c r="G327" s="33" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
     </row>
     <row r="328" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7142,7 +7135,7 @@
         <v>401</v>
       </c>
       <c r="F328" s="1" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
@@ -7172,10 +7165,10 @@
         <v>404</v>
       </c>
       <c r="F330" s="1" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B331" s="1" t="s">
         <v>405</v>
       </c>
@@ -7186,15 +7179,15 @@
         <v>814</v>
       </c>
       <c r="F331" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G331" s="33" t="s">
-        <v>541</v>
+        <v>522</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F332" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.25">
@@ -7208,16 +7201,16 @@
         <v>92</v>
       </c>
       <c r="F333" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G333" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A334" s="3"/>
       <c r="F334" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="335" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7232,10 +7225,10 @@
         <v>409</v>
       </c>
       <c r="F335" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G335" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
@@ -7250,10 +7243,10 @@
         <v>92113</v>
       </c>
       <c r="F336" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G336" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.25">
@@ -7268,10 +7261,10 @@
         <v>92119</v>
       </c>
       <c r="F337" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G337" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.25">
@@ -7286,10 +7279,10 @@
         <v>413</v>
       </c>
       <c r="F338" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G338" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="339" spans="1:7" x14ac:dyDescent="0.25">
@@ -7304,10 +7297,10 @@
         <v>923</v>
       </c>
       <c r="F339" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G339" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="340" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7322,10 +7315,10 @@
         <v>416</v>
       </c>
       <c r="F340" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G340" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.25">
@@ -7340,10 +7333,10 @@
         <v>418</v>
       </c>
       <c r="F341" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G341" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.25">
@@ -7357,15 +7350,15 @@
         <v>928</v>
       </c>
       <c r="F342" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="G342" s="33" t="s">
-        <v>542</v>
+        <v>523</v>
       </c>
     </row>
     <row r="343" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F343" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.25">
@@ -7382,14 +7375,14 @@
         <v>90919110</v>
       </c>
       <c r="G344" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B345" s="20"/>
       <c r="D345" s="3"/>
       <c r="F345" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.25">
@@ -7407,7 +7400,7 @@
         <v>90919110</v>
       </c>
       <c r="G346" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.25">
@@ -7425,7 +7418,7 @@
         <v>90919110</v>
       </c>
       <c r="G347" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="348" spans="1:7" x14ac:dyDescent="0.25">
@@ -7443,7 +7436,7 @@
         <v>90919110</v>
       </c>
       <c r="G348" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.25">
@@ -7461,7 +7454,7 @@
         <v>90919110</v>
       </c>
       <c r="G349" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
@@ -7478,7 +7471,7 @@
         <v>90919110</v>
       </c>
       <c r="G350" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
@@ -7495,7 +7488,7 @@
         <v>90919110</v>
       </c>
       <c r="G351" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.25">
@@ -7512,13 +7505,13 @@
         <v>90919110</v>
       </c>
       <c r="G352" s="33" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
     </row>
     <row r="353" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D353" s="3"/>
       <c r="F353" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="354" spans="2:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add 2 digit NAICS for summarizing later, update R file
</commit_message>
<xml_diff>
--- a/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
+++ b/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\GMacDonald\Documents\ipums-acs-naics-standardization\data\manual-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C1ACF4-D228-4A71-9F88-63CFE90CF334}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A748D6F6-4234-4FC2-A47F-4DBFDD4BF466}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15435" yWindow="45" windowWidth="9600" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017 Census Industry Code List" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="545">
   <si>
     <t>2017 Industry Code List</t>
   </si>
@@ -1669,6 +1669,15 @@
   </si>
   <si>
     <t>80000000-80811000-80812000-80813000</t>
+  </si>
+  <si>
+    <t>NAICS_2_Digit</t>
+  </si>
+  <si>
+    <t>Made decision to treat residuals as category minus everything else defined, for 2 digit made decision to treat as 33 similar to miscellaneous</t>
+  </si>
+  <si>
+    <t>Made decision to treat residuals as category minus everything else defined, could be 0, given other definitions and decisions made here, for 2 digit NAICS made arbitrary decision to assign to 44</t>
   </si>
 </sst>
 </file>
@@ -2139,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,19 +2165,19 @@
     <col min="9" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="C2" s="34"/>
       <c r="D2" s="12"/>
       <c r="F2" s="36"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="16" t="s">
         <v>1</v>
@@ -2185,14 +2194,17 @@
       <c r="G3" s="26" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="20" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="4" t="s">
         <v>434</v>
@@ -2200,13 +2212,13 @@
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
@@ -2223,11 +2235,11 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
@@ -2240,8 +2252,11 @@
       <c r="F9" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -2255,8 +2270,11 @@
       <c r="F11" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
@@ -2271,8 +2289,11 @@
       <c r="F12" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -2286,8 +2307,11 @@
       <c r="F13" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -2301,8 +2325,11 @@
       <c r="F14">
         <v>10113300</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="1" t="s">
         <v>18</v>
@@ -2316,8 +2343,11 @@
       <c r="F15" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
         <v>20</v>
@@ -2331,12 +2361,15 @@
       <c r="F16" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>22</v>
       </c>
@@ -2349,8 +2382,11 @@
       <c r="F18" s="1">
         <v>10210000</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="1" t="s">
         <v>24</v>
@@ -2364,8 +2400,11 @@
       <c r="F20">
         <v>10211000</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="1" t="s">
         <v>26</v>
@@ -2379,8 +2418,11 @@
       <c r="F21">
         <v>10212100</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="1" t="s">
         <v>28</v>
@@ -2394,8 +2436,11 @@
       <c r="F22">
         <v>10212200</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="1" t="s">
         <v>30</v>
@@ -2409,8 +2454,11 @@
       <c r="F23">
         <v>10212300</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H23" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
@@ -2427,8 +2475,11 @@
       <c r="G24" s="33" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="1" t="s">
         <v>35</v>
@@ -2442,8 +2493,11 @@
       <c r="F25">
         <v>10213000</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>37</v>
       </c>
@@ -2456,8 +2510,11 @@
       <c r="F27">
         <v>20000000</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H27" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="1" t="s">
         <v>39</v>
@@ -2472,8 +2529,11 @@
       <c r="F29">
         <v>20000000</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>40</v>
       </c>
@@ -2487,7 +2547,7 @@
         <v>30000000</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="1" t="s">
         <v>43</v>
@@ -2501,8 +2561,11 @@
       <c r="F33" s="37" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="1" t="s">
         <v>45</v>
@@ -2516,8 +2579,11 @@
       <c r="F34">
         <v>32311300</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H34" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="1" t="s">
         <v>46</v>
@@ -2531,8 +2597,11 @@
       <c r="F35">
         <v>32311400</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="1" t="s">
         <v>47</v>
@@ -2546,8 +2615,11 @@
       <c r="F36">
         <v>32311500</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="1" t="s">
         <v>48</v>
@@ -2561,8 +2633,11 @@
       <c r="F37">
         <v>32311600</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="1" t="s">
         <v>49</v>
@@ -2576,8 +2651,11 @@
       <c r="F38">
         <v>32311811</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H38" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>50</v>
@@ -2592,8 +2670,11 @@
       <c r="F39" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="1" t="s">
         <v>52</v>
@@ -2607,8 +2688,11 @@
       <c r="F40" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H40" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="1" t="s">
         <v>54</v>
@@ -2625,8 +2709,11 @@
       <c r="G41" s="33" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="1" t="s">
         <v>56</v>
@@ -2640,8 +2727,11 @@
       <c r="F42">
         <v>32329100</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="1" t="s">
         <v>57</v>
@@ -2658,8 +2748,11 @@
       <c r="G43" s="33" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="1" t="s">
         <v>58</v>
@@ -2676,8 +2769,11 @@
       <c r="G44" s="33" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="1" t="s">
         <v>59</v>
@@ -2694,8 +2790,11 @@
       <c r="G45" s="33" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="1" t="s">
         <v>61</v>
@@ -2712,8 +2811,11 @@
       <c r="G46" s="33" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="1" t="s">
         <v>62</v>
@@ -2730,8 +2832,11 @@
       <c r="G47" s="33" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="1" t="s">
         <v>63</v>
@@ -2748,8 +2853,11 @@
       <c r="G48" s="33" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="1" t="s">
         <v>65</v>
@@ -2766,8 +2874,11 @@
       <c r="G49" s="33" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H49" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="1" t="s">
         <v>67</v>
@@ -2784,8 +2895,11 @@
       <c r="G50" s="33" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="H50" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="1" t="s">
         <v>69</v>
@@ -2802,8 +2916,11 @@
       <c r="G51" s="33" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="H51" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="1" t="s">
         <v>70</v>
@@ -2820,8 +2937,11 @@
       <c r="G52" s="33" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="1" t="s">
         <v>72</v>
@@ -2835,8 +2955,11 @@
       <c r="F53" s="1">
         <v>32322100</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
         <v>73</v>
@@ -2850,8 +2973,11 @@
       <c r="F54" s="1">
         <v>32322210</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H54" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="1" t="s">
         <v>74</v>
@@ -2865,8 +2991,11 @@
       <c r="F55" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="1" t="s">
         <v>76</v>
@@ -2883,8 +3012,11 @@
       <c r="G56" s="33" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="1" t="s">
         <v>77</v>
@@ -2898,8 +3030,11 @@
       <c r="F57" s="1">
         <v>32324110</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="1" t="s">
         <v>78</v>
@@ -2913,8 +3048,11 @@
       <c r="F58">
         <v>32324190</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H58" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="1" t="s">
         <v>80</v>
@@ -2928,8 +3066,11 @@
       <c r="F59" s="1">
         <v>32325200</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="1" t="s">
         <v>81</v>
@@ -2943,8 +3084,11 @@
       <c r="F60" s="1">
         <v>32325300</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="1" t="s">
         <v>82</v>
@@ -2958,8 +3102,11 @@
       <c r="F61" s="1">
         <v>32325400</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="1" t="s">
         <v>83</v>
@@ -2973,8 +3120,11 @@
       <c r="F62" s="1">
         <v>32325500</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="1" t="s">
         <v>84</v>
@@ -2988,8 +3138,11 @@
       <c r="F63" s="1">
         <v>32325600</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="1" t="s">
         <v>85</v>
@@ -3002,6 +3155,9 @@
       </c>
       <c r="F64" s="1" t="s">
         <v>448</v>
+      </c>
+      <c r="H64" s="1">
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -3018,6 +3174,9 @@
       <c r="F65" s="1">
         <v>32326100</v>
       </c>
+      <c r="H65" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
@@ -3033,6 +3192,9 @@
       <c r="F66" s="1">
         <v>32326210</v>
       </c>
+      <c r="H66" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
@@ -3048,6 +3210,9 @@
       <c r="F67">
         <v>32326290</v>
       </c>
+      <c r="H67" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
@@ -3066,6 +3231,9 @@
       <c r="G68" s="33" t="s">
         <v>449</v>
       </c>
+      <c r="H68" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
@@ -3084,6 +3252,9 @@
       <c r="G69" s="33" t="s">
         <v>449</v>
       </c>
+      <c r="H69" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
@@ -3097,6 +3268,9 @@
       </c>
       <c r="F70" s="1">
         <v>31327200</v>
+      </c>
+      <c r="H70" s="1">
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3116,6 +3290,9 @@
       <c r="G71" s="33" t="s">
         <v>451</v>
       </c>
+      <c r="H71" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
@@ -3134,6 +3311,9 @@
       <c r="G72" s="33" t="s">
         <v>451</v>
       </c>
+      <c r="H72" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
@@ -3149,6 +3329,9 @@
       <c r="F73" s="1" t="s">
         <v>452</v>
       </c>
+      <c r="H73" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
@@ -3164,6 +3347,9 @@
       <c r="F74" s="1">
         <v>31331300</v>
       </c>
+      <c r="H74" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
@@ -3179,6 +3365,9 @@
       <c r="F75" s="1">
         <v>31331400</v>
       </c>
+      <c r="H75" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -3194,6 +3383,9 @@
       <c r="F76" s="1">
         <v>31331500</v>
       </c>
+      <c r="H76" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
@@ -3209,6 +3401,9 @@
       <c r="F77" s="1">
         <v>31332100</v>
       </c>
+      <c r="H77" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
@@ -3226,6 +3421,9 @@
         <v>31332200</v>
       </c>
       <c r="G78" s="33"/>
+      <c r="H78" s="1">
+        <v>33</v>
+      </c>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
@@ -3246,6 +3444,9 @@
         <v>453</v>
       </c>
       <c r="G79" s="33"/>
+      <c r="H79" s="1">
+        <v>33</v>
+      </c>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
@@ -3266,6 +3467,9 @@
         <v>31332700</v>
       </c>
       <c r="G80" s="33"/>
+      <c r="H80" s="1">
+        <v>33</v>
+      </c>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
@@ -3286,6 +3490,9 @@
         <v>31332800</v>
       </c>
       <c r="G81" s="33"/>
+      <c r="H81" s="1">
+        <v>33</v>
+      </c>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
@@ -3308,6 +3515,9 @@
       <c r="G82" s="33" t="s">
         <v>454</v>
       </c>
+      <c r="H82" s="1">
+        <v>33</v>
+      </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
@@ -3330,6 +3540,9 @@
       <c r="G83" s="33" t="s">
         <v>454</v>
       </c>
+      <c r="H83" s="1">
+        <v>33</v>
+      </c>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
@@ -3352,6 +3565,9 @@
       <c r="G84" s="33" t="s">
         <v>530</v>
       </c>
+      <c r="H84" s="1">
+        <v>33</v>
+      </c>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
@@ -3372,6 +3588,9 @@
         <v>31333110</v>
       </c>
       <c r="G85" s="33"/>
+      <c r="H85" s="1">
+        <v>33</v>
+      </c>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
@@ -3392,6 +3611,9 @@
         <v>456</v>
       </c>
       <c r="G86" s="33"/>
+      <c r="H86" s="1">
+        <v>33</v>
+      </c>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
@@ -3412,6 +3634,9 @@
         <v>31333300</v>
       </c>
       <c r="G87" s="33"/>
+      <c r="H87" s="1">
+        <v>33</v>
+      </c>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
@@ -3432,6 +3657,9 @@
         <v>31333500</v>
       </c>
       <c r="G88" s="33"/>
+      <c r="H88" s="1">
+        <v>33</v>
+      </c>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
@@ -3452,6 +3680,9 @@
         <v>31333600</v>
       </c>
       <c r="G89" s="33"/>
+      <c r="H89" s="1">
+        <v>33</v>
+      </c>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
@@ -3474,6 +3705,9 @@
       <c r="G90" s="33" t="s">
         <v>533</v>
       </c>
+      <c r="H90" s="1">
+        <v>33</v>
+      </c>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
@@ -3494,6 +3728,9 @@
         <v>31334100</v>
       </c>
       <c r="G91" s="33"/>
+      <c r="H91" s="1">
+        <v>33</v>
+      </c>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
@@ -3516,6 +3753,9 @@
       <c r="G92" s="33" t="s">
         <v>458</v>
       </c>
+      <c r="H92" s="1">
+        <v>33</v>
+      </c>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
@@ -3536,6 +3776,9 @@
         <v>31334500</v>
       </c>
       <c r="G93" s="33"/>
+      <c r="H93" s="1">
+        <v>33</v>
+      </c>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
@@ -3558,6 +3801,9 @@
       <c r="G94" s="33" t="s">
         <v>458</v>
       </c>
+      <c r="H94" s="1">
+        <v>33</v>
+      </c>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
@@ -3578,6 +3824,9 @@
         <v>31335200</v>
       </c>
       <c r="G95" s="33"/>
+      <c r="H95" s="1">
+        <v>33</v>
+      </c>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
@@ -3597,6 +3846,9 @@
         <v>459</v>
       </c>
       <c r="G96" s="33"/>
+      <c r="H96" s="1">
+        <v>33</v>
+      </c>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
@@ -3617,6 +3869,9 @@
         <v>460</v>
       </c>
       <c r="G97" s="33"/>
+      <c r="H97" s="1">
+        <v>33</v>
+      </c>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
@@ -3637,6 +3892,9 @@
         <v>461</v>
       </c>
       <c r="G98" s="33"/>
+      <c r="H98" s="1">
+        <v>33</v>
+      </c>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
@@ -3657,6 +3915,9 @@
         <v>31336419</v>
       </c>
       <c r="G99" s="33"/>
+      <c r="H99" s="1">
+        <v>33</v>
+      </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
@@ -3679,6 +3940,9 @@
       <c r="G100" s="33" t="s">
         <v>462</v>
       </c>
+      <c r="H100" s="1">
+        <v>33</v>
+      </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
@@ -3699,6 +3963,9 @@
         <v>31336600</v>
       </c>
       <c r="G101" s="33"/>
+      <c r="H101" s="1">
+        <v>33</v>
+      </c>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
@@ -3721,6 +3988,9 @@
       <c r="G102" s="33" t="s">
         <v>462</v>
       </c>
+      <c r="H102" s="1">
+        <v>33</v>
+      </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
@@ -3741,6 +4011,9 @@
         <v>31321100</v>
       </c>
       <c r="G103" s="33"/>
+      <c r="H103" s="1">
+        <v>32</v>
+      </c>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
@@ -3761,6 +4034,9 @@
         <v>31321200</v>
       </c>
       <c r="G104" s="33"/>
+      <c r="H104" s="1">
+        <v>32</v>
+      </c>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
@@ -3783,6 +4059,9 @@
       <c r="G105" s="33" t="s">
         <v>463</v>
       </c>
+      <c r="H105" s="1">
+        <v>32</v>
+      </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
@@ -3805,6 +4084,9 @@
       <c r="G106" s="33" t="s">
         <v>465</v>
       </c>
+      <c r="H106" s="1">
+        <v>32</v>
+      </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
@@ -3823,6 +4105,9 @@
       <c r="F107" s="1">
         <v>31337000</v>
       </c>
+      <c r="H107" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
@@ -3838,6 +4123,9 @@
       <c r="F108" s="1">
         <v>31339100</v>
       </c>
+      <c r="H108" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="109" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
@@ -3856,6 +4144,9 @@
       <c r="G109" s="33" t="s">
         <v>466</v>
       </c>
+      <c r="H109" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="110" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
@@ -3874,6 +4165,9 @@
       <c r="G110" s="33" t="s">
         <v>468</v>
       </c>
+      <c r="H110" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="111" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
@@ -3890,13 +4184,16 @@
         <v>536</v>
       </c>
       <c r="G111" s="33" t="s">
-        <v>530</v>
+        <v>543</v>
+      </c>
+      <c r="H111" s="1">
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D112" s="3"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
         <v>153</v>
       </c>
@@ -3909,14 +4206,17 @@
       <c r="F113" s="1">
         <v>41420000</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H113" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="F114" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="1" t="s">
         <v>155</v>
@@ -3931,8 +4231,11 @@
       <c r="F115" s="1">
         <v>41423100</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H115" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
       <c r="B116" s="1" t="s">
         <v>156</v>
@@ -3947,8 +4250,11 @@
       <c r="F116" s="1">
         <v>41423200</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H116" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
       <c r="B117" s="1" t="s">
         <v>157</v>
@@ -3963,8 +4269,11 @@
       <c r="F117" s="1">
         <v>41423300</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H117" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
       <c r="B118" s="1" t="s">
         <v>158</v>
@@ -3979,8 +4288,11 @@
       <c r="F118" s="1">
         <v>41423400</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H118" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
       <c r="B119" s="1" t="s">
         <v>159</v>
@@ -3995,8 +4307,11 @@
       <c r="F119" s="1">
         <v>41423500</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H119" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="1" t="s">
         <v>160</v>
@@ -4011,8 +4326,11 @@
       <c r="F120" s="1">
         <v>41423600</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H120" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
       <c r="B121" s="1" t="s">
         <v>161</v>
@@ -4027,8 +4345,11 @@
       <c r="F121" s="1">
         <v>41423700</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H121" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="1" t="s">
         <v>162</v>
@@ -4043,8 +4364,11 @@
       <c r="F122" s="1">
         <v>41423800</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H122" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="1" t="s">
         <v>163</v>
@@ -4059,8 +4383,11 @@
       <c r="F123" s="1">
         <v>41423930</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H123" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="1" t="s">
         <v>164</v>
@@ -4075,8 +4402,11 @@
       <c r="F124" s="1" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H124" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="1" t="s">
         <v>166</v>
@@ -4091,8 +4421,11 @@
       <c r="F125" s="1">
         <v>41424100</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H125" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="1" t="s">
         <v>167</v>
@@ -4107,8 +4440,11 @@
       <c r="F126" s="1" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H126" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="1" t="s">
         <v>169</v>
@@ -4123,8 +4459,11 @@
       <c r="F127" s="1">
         <v>41424300</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H127" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="1" t="s">
         <v>170</v>
@@ -4139,8 +4478,11 @@
       <c r="F128" s="1">
         <v>41424400</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H128" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="6"/>
       <c r="B129" s="1" t="s">
         <v>171</v>
@@ -4155,8 +4497,11 @@
       <c r="F129" s="1">
         <v>41424500</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H129" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="1" t="s">
         <v>172</v>
@@ -4171,8 +4516,11 @@
       <c r="F130" s="1">
         <v>41424700</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H130" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="1" t="s">
         <v>173</v>
@@ -4187,8 +4535,11 @@
       <c r="F131" s="1">
         <v>41424800</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H131" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="1" t="s">
         <v>174</v>
@@ -4203,8 +4554,11 @@
       <c r="F132" s="1">
         <v>41424910</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H132" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
       <c r="B133" s="1" t="s">
         <v>175</v>
@@ -4219,8 +4573,11 @@
       <c r="F133" s="1" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H133" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="1" t="s">
         <v>177</v>
@@ -4238,8 +4595,11 @@
       <c r="G134" s="33" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H134" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="s">
         <v>178</v>
       </c>
@@ -4256,13 +4616,16 @@
       <c r="G135" s="33" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H135" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F136" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
         <v>180</v>
       </c>
@@ -4276,13 +4639,13 @@
         <v>42000000</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="F138" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="1" t="s">
         <v>183</v>
@@ -4296,8 +4659,11 @@
       <c r="F139" s="1">
         <v>42441100</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H139" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="1" t="s">
         <v>184</v>
@@ -4311,8 +4677,11 @@
       <c r="F140" s="1">
         <v>42441200</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H140" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="1" t="s">
         <v>185</v>
@@ -4326,8 +4695,11 @@
       <c r="F141" s="1">
         <v>42441300</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H141" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="1" t="s">
         <v>186</v>
@@ -4341,8 +4713,11 @@
       <c r="F142" s="1">
         <v>42442000</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H142" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="1" t="s">
         <v>187</v>
@@ -4356,8 +4731,11 @@
       <c r="F143" s="1">
         <v>42443141</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H143" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="1" t="s">
         <v>188</v>
@@ -4371,8 +4749,11 @@
       <c r="F144" s="1">
         <v>42443142</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H144" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="1" t="s">
         <v>189</v>
@@ -4386,8 +4767,11 @@
       <c r="F145" s="1" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H145" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="1" t="s">
         <v>191</v>
@@ -4401,8 +4785,11 @@
       <c r="F146" s="1">
         <v>42444130</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H146" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="1" t="s">
         <v>192</v>
@@ -4416,8 +4803,11 @@
       <c r="F147" s="1">
         <v>42444200</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H147" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="1" t="s">
         <v>430</v>
@@ -4431,8 +4821,11 @@
       <c r="F148" s="1">
         <v>42445110</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H148" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="1" t="s">
         <v>193</v>
@@ -4446,8 +4839,11 @@
       <c r="F149" s="1">
         <v>42445120</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H149" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="1" t="s">
         <v>194</v>
@@ -4461,8 +4857,11 @@
       <c r="F150" s="1">
         <v>42445200</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H150" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="1" t="s">
         <v>195</v>
@@ -4476,8 +4875,11 @@
       <c r="F151" s="1">
         <v>42445300</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H151" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="1" t="s">
         <v>196</v>
@@ -4491,8 +4893,11 @@
       <c r="F152" s="1">
         <v>42446110</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H152" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="1" t="s">
         <v>197</v>
@@ -4506,8 +4911,11 @@
       <c r="F153" s="1" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H153" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="1" t="s">
         <v>199</v>
@@ -4521,8 +4929,11 @@
       <c r="F154" s="1">
         <v>42447000</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H154" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="1" t="s">
         <v>200</v>
@@ -4536,8 +4947,11 @@
       <c r="F155" s="1">
         <v>42448100</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H155" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="1" t="s">
         <v>201</v>
@@ -4554,8 +4968,11 @@
       <c r="G156" s="33" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H156" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="1" t="s">
         <v>202</v>
@@ -4569,8 +4986,11 @@
       <c r="F157" s="1">
         <v>42448300</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H157" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="1" t="s">
         <v>203</v>
@@ -4584,8 +5004,11 @@
       <c r="F158" s="1" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H158" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="1" t="s">
         <v>205</v>
@@ -4599,8 +5022,11 @@
       <c r="F159" s="1">
         <v>42451130</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H159" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="1" t="s">
         <v>206</v>
@@ -4613,6 +5039,9 @@
       </c>
       <c r="F160" s="1">
         <v>42451140</v>
+      </c>
+      <c r="H160" s="1">
+        <v>45</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
@@ -4632,6 +5061,9 @@
       <c r="G161" s="33" t="s">
         <v>477</v>
       </c>
+      <c r="H161" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
@@ -4650,6 +5082,9 @@
       <c r="G162" s="33" t="s">
         <v>478</v>
       </c>
+      <c r="H162" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="163" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
@@ -4665,6 +5100,9 @@
       <c r="F163" s="1">
         <v>42452300</v>
       </c>
+      <c r="H163" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
@@ -4680,6 +5118,9 @@
       <c r="F164" s="1">
         <v>42453100</v>
       </c>
+      <c r="H164" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="165" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
@@ -4697,6 +5138,9 @@
         <v>42453210</v>
       </c>
       <c r="G165" s="33"/>
+      <c r="H165" s="1">
+        <v>45</v>
+      </c>
       <c r="I165" s="7"/>
       <c r="J165" s="7"/>
       <c r="K165" s="7"/>
@@ -4717,6 +5161,9 @@
         <v>42453300</v>
       </c>
       <c r="G166" s="33"/>
+      <c r="H166" s="1">
+        <v>45</v>
+      </c>
       <c r="I166" s="7"/>
       <c r="J166" s="7"/>
       <c r="K166" s="7"/>
@@ -4737,6 +5184,9 @@
         <v>42453220</v>
       </c>
       <c r="G167" s="33"/>
+      <c r="H167" s="1">
+        <v>45</v>
+      </c>
       <c r="I167" s="7"/>
       <c r="J167" s="7"/>
       <c r="K167" s="7"/>
@@ -4757,6 +5207,9 @@
         <v>42453900</v>
       </c>
       <c r="G168" s="33"/>
+      <c r="H168" s="1">
+        <v>45</v>
+      </c>
       <c r="I168" s="7"/>
       <c r="J168" s="7"/>
       <c r="K168" s="7"/>
@@ -4779,6 +5232,9 @@
       <c r="G169" s="33" t="s">
         <v>480</v>
       </c>
+      <c r="H169" s="1">
+        <v>45</v>
+      </c>
       <c r="I169" s="7"/>
       <c r="J169" s="7"/>
       <c r="K169" s="7"/>
@@ -4799,6 +5255,9 @@
         <v>42454200</v>
       </c>
       <c r="G170" s="33"/>
+      <c r="H170" s="1">
+        <v>45</v>
+      </c>
       <c r="I170" s="7"/>
       <c r="J170" s="7"/>
       <c r="K170" s="7"/>
@@ -4821,6 +5280,9 @@
       <c r="G171" s="33" t="s">
         <v>481</v>
       </c>
+      <c r="H171" s="1">
+        <v>45</v>
+      </c>
       <c r="I171" s="7"/>
       <c r="J171" s="7"/>
       <c r="K171" s="7"/>
@@ -4841,6 +5303,9 @@
         <v>42454390</v>
       </c>
       <c r="G172" s="33"/>
+      <c r="H172" s="1">
+        <v>45</v>
+      </c>
       <c r="I172" s="7"/>
       <c r="J172" s="7"/>
       <c r="K172" s="7"/>
@@ -4861,7 +5326,10 @@
         <v>538</v>
       </c>
       <c r="G173" s="33" t="s">
-        <v>539</v>
+        <v>544</v>
+      </c>
+      <c r="H173" s="1">
+        <v>44</v>
       </c>
       <c r="I173" s="7"/>
       <c r="J173" s="7"/>
@@ -4944,6 +5412,9 @@
       <c r="F179" s="1">
         <v>43481000</v>
       </c>
+      <c r="H179" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
@@ -4959,6 +5430,9 @@
       <c r="F180" s="1">
         <v>43482000</v>
       </c>
+      <c r="H180" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
@@ -4974,6 +5448,9 @@
       <c r="F181" s="1">
         <v>43483000</v>
       </c>
+      <c r="H181" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
@@ -4989,6 +5466,9 @@
       <c r="F182" s="1">
         <v>43484000</v>
       </c>
+      <c r="H182" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="183" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
@@ -5004,6 +5484,9 @@
       <c r="F183" s="1" t="s">
         <v>483</v>
       </c>
+      <c r="H183" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
@@ -5019,6 +5502,9 @@
       <c r="F184" s="1">
         <v>43485300</v>
       </c>
+      <c r="H184" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
@@ -5034,6 +5520,9 @@
       <c r="F185" s="1">
         <v>43486000</v>
       </c>
+      <c r="H185" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
@@ -5049,6 +5538,9 @@
       <c r="F186" s="1">
         <v>43487000</v>
       </c>
+      <c r="H186" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
@@ -5064,6 +5556,9 @@
       <c r="F187" s="1">
         <v>43488000</v>
       </c>
+      <c r="H187" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
@@ -5082,6 +5577,9 @@
       <c r="G188" s="33" t="s">
         <v>484</v>
       </c>
+      <c r="H188" s="1">
+        <v>49</v>
+      </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
@@ -5097,6 +5595,9 @@
       <c r="F189" s="1">
         <v>43492000</v>
       </c>
+      <c r="H189" s="1">
+        <v>49</v>
+      </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
@@ -5112,6 +5613,9 @@
       <c r="F190" s="1">
         <v>43493000</v>
       </c>
+      <c r="H190" s="1">
+        <v>49</v>
+      </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D191" s="3"/>
@@ -5132,6 +5636,9 @@
       <c r="F192" s="1">
         <v>44220000</v>
       </c>
+      <c r="H192" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="11"/>
@@ -5155,6 +5662,9 @@
         <v>44221100</v>
       </c>
       <c r="G194" s="33"/>
+      <c r="H194" s="1">
+        <v>22</v>
+      </c>
       <c r="I194" s="7"/>
       <c r="J194" s="7"/>
       <c r="K194" s="7"/>
@@ -5175,6 +5685,9 @@
         <v>44221200</v>
       </c>
       <c r="G195" s="33"/>
+      <c r="H195" s="1">
+        <v>22</v>
+      </c>
       <c r="I195" s="7"/>
       <c r="J195" s="7"/>
       <c r="K195" s="7"/>
@@ -5195,6 +5708,9 @@
         <v>436</v>
       </c>
       <c r="G196" s="33"/>
+      <c r="H196" s="1">
+        <v>22</v>
+      </c>
       <c r="I196" s="7"/>
       <c r="J196" s="7"/>
       <c r="K196" s="7"/>
@@ -5217,6 +5733,9 @@
       <c r="G197" s="33" t="s">
         <v>485</v>
       </c>
+      <c r="H197" s="1">
+        <v>22</v>
+      </c>
       <c r="I197" s="7"/>
       <c r="J197" s="7"/>
       <c r="K197" s="7"/>
@@ -5239,6 +5758,9 @@
       <c r="G198" s="33" t="s">
         <v>485</v>
       </c>
+      <c r="H198" s="1">
+        <v>22</v>
+      </c>
       <c r="I198" s="7"/>
       <c r="J198" s="7"/>
       <c r="K198" s="7"/>
@@ -5261,6 +5783,9 @@
       <c r="G199" s="33" t="s">
         <v>539</v>
       </c>
+      <c r="H199" s="1">
+        <v>22</v>
+      </c>
       <c r="I199" s="7"/>
       <c r="J199" s="7"/>
       <c r="K199" s="7"/>
@@ -5285,6 +5810,9 @@
         <v>50000000</v>
       </c>
       <c r="G201" s="33"/>
+      <c r="H201" s="1">
+        <v>51</v>
+      </c>
       <c r="I201" s="7"/>
       <c r="J201" s="7"/>
       <c r="K201" s="7"/>
@@ -5318,6 +5846,9 @@
         <v>50511110</v>
       </c>
       <c r="G203" s="33"/>
+      <c r="H203" s="1">
+        <v>51</v>
+      </c>
       <c r="I203" s="7"/>
       <c r="J203" s="7"/>
       <c r="K203" s="7"/>
@@ -5338,6 +5869,9 @@
         <v>486</v>
       </c>
       <c r="G204" s="33"/>
+      <c r="H204" s="1">
+        <v>51</v>
+      </c>
       <c r="I204" s="7"/>
       <c r="J204" s="7"/>
       <c r="K204" s="7"/>
@@ -5358,6 +5892,9 @@
         <v>50511200</v>
       </c>
       <c r="G205" s="33"/>
+      <c r="H205" s="1">
+        <v>51</v>
+      </c>
       <c r="I205" s="7"/>
       <c r="J205" s="7"/>
       <c r="K205" s="7"/>
@@ -5380,6 +5917,9 @@
       <c r="G206" s="33" t="s">
         <v>487</v>
       </c>
+      <c r="H206" s="1">
+        <v>51</v>
+      </c>
       <c r="I206" s="7"/>
       <c r="J206" s="7"/>
       <c r="K206" s="7"/>
@@ -5402,6 +5942,9 @@
       <c r="G207" s="33" t="s">
         <v>487</v>
       </c>
+      <c r="H207" s="1">
+        <v>51</v>
+      </c>
       <c r="I207" s="7"/>
       <c r="J207" s="7"/>
       <c r="K207" s="7"/>
@@ -5422,6 +5965,9 @@
         <v>50515000</v>
       </c>
       <c r="G208" s="33"/>
+      <c r="H208" s="1">
+        <v>51</v>
+      </c>
       <c r="I208" s="7"/>
       <c r="J208" s="7"/>
       <c r="K208" s="7"/>
@@ -5442,6 +5988,9 @@
         <v>50519130</v>
       </c>
       <c r="G209" s="33"/>
+      <c r="H209" s="1">
+        <v>51</v>
+      </c>
       <c r="I209" s="7"/>
       <c r="J209" s="7"/>
       <c r="K209" s="7"/>
@@ -5462,6 +6011,9 @@
         <v>50517311</v>
       </c>
       <c r="G210" s="33"/>
+      <c r="H210" s="1">
+        <v>51</v>
+      </c>
       <c r="I210" s="7"/>
       <c r="J210" s="7"/>
       <c r="K210" s="7"/>
@@ -5481,6 +6033,9 @@
       <c r="F211" s="1" t="s">
         <v>488</v>
       </c>
+      <c r="H211" s="1">
+        <v>51</v>
+      </c>
       <c r="I211" s="1"/>
       <c r="J211" s="1"/>
     </row>
@@ -5502,6 +6057,9 @@
       <c r="G212" s="33" t="s">
         <v>489</v>
       </c>
+      <c r="H212" s="1">
+        <v>51</v>
+      </c>
       <c r="I212" s="7"/>
       <c r="J212" s="7"/>
       <c r="K212" s="7"/>
@@ -5524,6 +6082,9 @@
       <c r="G213" s="33" t="s">
         <v>490</v>
       </c>
+      <c r="H213" s="1">
+        <v>51</v>
+      </c>
       <c r="I213" s="7"/>
       <c r="J213" s="7"/>
       <c r="K213" s="7"/>
@@ -5545,6 +6106,9 @@
       </c>
       <c r="G214" s="33" t="s">
         <v>490</v>
+      </c>
+      <c r="H214" s="1">
+        <v>51</v>
       </c>
       <c r="I214" s="7"/>
       <c r="J214" s="7"/>
@@ -5612,6 +6176,9 @@
         <v>55520000</v>
       </c>
       <c r="G218" s="33"/>
+      <c r="H218" s="1">
+        <v>52</v>
+      </c>
       <c r="I218" s="7"/>
       <c r="J218" s="7"/>
       <c r="K218" s="7"/>
@@ -5647,6 +6214,9 @@
       <c r="G220" s="33" t="s">
         <v>493</v>
       </c>
+      <c r="H220" s="1">
+        <v>52</v>
+      </c>
       <c r="I220" s="7"/>
       <c r="J220" s="7"/>
       <c r="K220" s="7"/>
@@ -5669,6 +6239,9 @@
       <c r="G221" s="33" t="s">
         <v>493</v>
       </c>
+      <c r="H221" s="1">
+        <v>52</v>
+      </c>
       <c r="I221" s="7"/>
       <c r="J221" s="7"/>
       <c r="K221" s="7"/>
@@ -5687,6 +6260,9 @@
       <c r="F222" s="1" t="s">
         <v>494</v>
       </c>
+      <c r="H222" s="1">
+        <v>52</v>
+      </c>
     </row>
     <row r="223" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" s="3"/>
@@ -5702,6 +6278,9 @@
       <c r="F223" s="1">
         <v>55523000</v>
       </c>
+      <c r="H223" s="1">
+        <v>52</v>
+      </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B224" s="1" t="s">
@@ -5716,8 +6295,11 @@
       <c r="F224" s="1">
         <v>55524100</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H224" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B225" s="1" t="s">
         <v>287</v>
       </c>
@@ -5730,13 +6312,16 @@
       <c r="F225" s="1">
         <v>55524200</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H225" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F226" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B227" s="30" t="s">
         <v>288</v>
       </c>
@@ -5749,14 +6334,17 @@
       <c r="F227" s="1">
         <v>55530000</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H227" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
       <c r="F228" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A229" s="3"/>
       <c r="B229" s="1" t="s">
         <v>290</v>
@@ -5770,8 +6358,11 @@
       <c r="F229" s="1" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H229" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" s="3"/>
       <c r="B230" s="1" t="s">
         <v>292</v>
@@ -5785,15 +6376,21 @@
       <c r="F230" s="1">
         <v>55531300</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H230" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="3"/>
       <c r="D231" s="3"/>
       <c r="F231" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H231" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="3"/>
       <c r="B232" s="1" t="s">
         <v>293</v>
@@ -5807,8 +6404,11 @@
       <c r="F232" s="1">
         <v>55532100</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H232" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A233" s="6"/>
       <c r="B233" s="1" t="s">
         <v>294</v>
@@ -5825,8 +6425,11 @@
       <c r="G233" s="33" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H233" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B234" s="1" t="s">
         <v>296</v>
       </c>
@@ -5839,13 +6442,16 @@
       <c r="F234" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H234" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F235" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="8" t="s">
         <v>298</v>
       </c>
@@ -5861,7 +6467,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="8" t="s">
         <v>301</v>
       </c>
@@ -5873,13 +6479,13 @@
         <v>441</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D238" s="3"/>
       <c r="F238" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B239" s="30" t="s">
         <v>302</v>
       </c>
@@ -5892,8 +6498,11 @@
       <c r="F239" s="1">
         <v>60540000</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H239" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="F240" s="1" t="s">
         <v>441</v>
@@ -5913,6 +6522,9 @@
       <c r="F241" s="1">
         <v>60541100</v>
       </c>
+      <c r="H241" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="242" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
@@ -5928,6 +6540,9 @@
       <c r="F242" s="1">
         <v>60541200</v>
       </c>
+      <c r="H242" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
@@ -5943,6 +6558,9 @@
       <c r="F243" s="1">
         <v>60541300</v>
       </c>
+      <c r="H243" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
@@ -5958,6 +6576,9 @@
       <c r="F244" s="1">
         <v>60541400</v>
       </c>
+      <c r="H244" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="245" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
@@ -5975,6 +6596,9 @@
         <v>60541500</v>
       </c>
       <c r="G245" s="33"/>
+      <c r="H245" s="1">
+        <v>54</v>
+      </c>
       <c r="I245" s="7"/>
       <c r="J245" s="7"/>
       <c r="K245" s="7"/>
@@ -5995,6 +6619,9 @@
         <v>60541600</v>
       </c>
       <c r="G246" s="33"/>
+      <c r="H246" s="1">
+        <v>54</v>
+      </c>
       <c r="I246" s="7"/>
       <c r="J246" s="7"/>
       <c r="K246" s="7"/>
@@ -6015,6 +6642,9 @@
         <v>60541700</v>
       </c>
       <c r="G247" s="33"/>
+      <c r="H247" s="1">
+        <v>54</v>
+      </c>
       <c r="I247" s="7"/>
       <c r="J247" s="7"/>
       <c r="K247" s="7"/>
@@ -6035,6 +6665,9 @@
         <v>60541800</v>
       </c>
       <c r="G248" s="33"/>
+      <c r="H248" s="1">
+        <v>54</v>
+      </c>
       <c r="I248" s="7"/>
       <c r="J248" s="7"/>
       <c r="K248" s="7"/>
@@ -6055,6 +6688,9 @@
         <v>60541940</v>
       </c>
       <c r="G249" s="33"/>
+      <c r="H249" s="1">
+        <v>54</v>
+      </c>
       <c r="I249" s="7"/>
       <c r="J249" s="7"/>
       <c r="K249" s="7"/>
@@ -6075,6 +6711,9 @@
         <v>500</v>
       </c>
       <c r="G250" s="33"/>
+      <c r="H250" s="1">
+        <v>54</v>
+      </c>
       <c r="I250" s="7"/>
       <c r="J250" s="7"/>
       <c r="K250" s="7"/>
@@ -6100,6 +6739,9 @@
         <v>60550000</v>
       </c>
       <c r="G252" s="33"/>
+      <c r="H252" s="1">
+        <v>55</v>
+      </c>
       <c r="I252" s="7"/>
       <c r="J252" s="7"/>
       <c r="K252" s="7"/>
@@ -6133,6 +6775,9 @@
         <v>60550000</v>
       </c>
       <c r="G254" s="33"/>
+      <c r="H254" s="1">
+        <v>55</v>
+      </c>
       <c r="I254" s="7"/>
       <c r="J254" s="7"/>
       <c r="K254" s="7"/>
@@ -6166,18 +6811,21 @@
         <v>60560000</v>
       </c>
       <c r="G256" s="33"/>
+      <c r="H256" s="1">
+        <v>56</v>
+      </c>
       <c r="I256" s="7"/>
       <c r="J256" s="7"/>
       <c r="K256" s="7"/>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="3"/>
       <c r="D257" s="3"/>
       <c r="F257" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="3"/>
       <c r="B258" s="1" t="s">
         <v>319</v>
@@ -6191,8 +6839,11 @@
       <c r="F258" s="1">
         <v>60561300</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H258" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="3"/>
       <c r="B259" s="1" t="s">
         <v>320</v>
@@ -6206,8 +6857,11 @@
       <c r="F259" s="1">
         <v>60561400</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H259" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="3"/>
       <c r="B260" s="1" t="s">
         <v>321</v>
@@ -6221,8 +6875,11 @@
       <c r="F260" s="1">
         <v>60561500</v>
       </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H260" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="6"/>
       <c r="B261" s="1" t="s">
         <v>322</v>
@@ -6236,8 +6893,11 @@
       <c r="F261" s="1">
         <v>60561600</v>
       </c>
-    </row>
-    <row r="262" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H261" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="3"/>
       <c r="B262" s="1" t="s">
         <v>323</v>
@@ -6252,8 +6912,11 @@
       <c r="F262" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H262" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="3"/>
       <c r="B263" s="1" t="s">
         <v>325</v>
@@ -6267,8 +6930,11 @@
       <c r="F263" s="1">
         <v>60561730</v>
       </c>
-    </row>
-    <row r="264" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H263" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A264" s="3"/>
       <c r="B264" s="1" t="s">
         <v>326</v>
@@ -6282,8 +6948,11 @@
       <c r="F264" s="1" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H264" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B265" s="1" t="s">
         <v>328</v>
       </c>
@@ -6296,13 +6965,16 @@
       <c r="F265" s="1">
         <v>60562000</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H265" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F266" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="8" t="s">
         <v>329</v>
       </c>
@@ -6317,13 +6989,13 @@
         <v>503</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D268" s="3"/>
       <c r="F268" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B269" s="30" t="s">
         <v>332</v>
       </c>
@@ -6337,14 +7009,17 @@
       <c r="F269" s="1">
         <v>65610000</v>
       </c>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H269" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="3"/>
       <c r="F270" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="3"/>
       <c r="B271" s="1" t="s">
         <v>334</v>
@@ -6358,8 +7033,11 @@
       <c r="F271" s="1">
         <v>65611100</v>
       </c>
-    </row>
-    <row r="272" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H271" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="3"/>
       <c r="B272" s="1" t="s">
         <v>335</v>
@@ -6373,8 +7051,11 @@
       <c r="F272" s="1" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H272" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="3"/>
       <c r="B273" s="1" t="s">
         <v>337</v>
@@ -6388,8 +7069,11 @@
       <c r="F273" s="1" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="274" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H273" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B274" s="1" t="s">
         <v>339</v>
       </c>
@@ -6402,13 +7086,16 @@
       <c r="F274" s="1" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H274" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F275" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B276" s="30" t="s">
         <v>341</v>
       </c>
@@ -6422,14 +7109,17 @@
       <c r="F276" s="1">
         <v>65620000</v>
       </c>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H276" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="3"/>
       <c r="F277" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="3"/>
       <c r="B278" s="1" t="s">
         <v>343</v>
@@ -6443,8 +7133,11 @@
       <c r="F278" s="1">
         <v>65621100</v>
       </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H278" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="3"/>
       <c r="B279" s="1" t="s">
         <v>344</v>
@@ -6458,8 +7151,11 @@
       <c r="F279" s="1">
         <v>65621200</v>
       </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H279" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="3"/>
       <c r="B280" s="1" t="s">
         <v>345</v>
@@ -6473,8 +7169,11 @@
       <c r="F280" s="1">
         <v>65621310</v>
       </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H280" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="2"/>
       <c r="B281" s="1" t="s">
         <v>346</v>
@@ -6488,8 +7187,11 @@
       <c r="F281" s="1">
         <v>65621320</v>
       </c>
-    </row>
-    <row r="282" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H281" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="3"/>
       <c r="B282" s="1" t="s">
         <v>347</v>
@@ -6504,8 +7206,11 @@
       <c r="F282" s="1" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H282" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="3"/>
       <c r="B283" s="1" t="s">
         <v>349</v>
@@ -6519,8 +7224,11 @@
       <c r="F283" s="1">
         <v>65621400</v>
       </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H283" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284" s="3"/>
       <c r="B284" s="1" t="s">
         <v>350</v>
@@ -6534,8 +7242,11 @@
       <c r="F284" s="1">
         <v>65621600</v>
       </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H284" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285" s="3"/>
       <c r="B285" s="1" t="s">
         <v>351</v>
@@ -6549,8 +7260,11 @@
       <c r="F285" s="1" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="286" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H285" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A286" s="3"/>
       <c r="B286" s="1" t="s">
         <v>433</v>
@@ -6564,8 +7278,11 @@
       <c r="F286" s="1" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H286" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287" s="3"/>
       <c r="B287" s="1" t="s">
         <v>354</v>
@@ -6579,8 +7296,11 @@
       <c r="F287" s="1">
         <v>65622200</v>
       </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H287" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="3"/>
       <c r="B288" s="1" t="s">
         <v>355</v>
@@ -6594,8 +7314,11 @@
       <c r="F288" s="1">
         <v>65623100</v>
       </c>
-    </row>
-    <row r="289" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H288" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="3"/>
       <c r="B289" s="1" t="s">
         <v>356</v>
@@ -6609,8 +7332,11 @@
       <c r="F289" s="1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H289" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="3"/>
       <c r="B290" s="1" t="s">
         <v>358</v>
@@ -6624,8 +7350,11 @@
       <c r="F290" s="1">
         <v>65624100</v>
       </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H290" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="3"/>
       <c r="B291" s="1" t="s">
         <v>359</v>
@@ -6639,8 +7368,11 @@
       <c r="F291" s="1">
         <v>65624200</v>
       </c>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H291" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="3"/>
       <c r="B292" s="1" t="s">
         <v>360</v>
@@ -6654,8 +7386,11 @@
       <c r="F292" s="1">
         <v>65624300</v>
       </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H292" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B293" s="1" t="s">
         <v>361</v>
       </c>
@@ -6668,13 +7403,16 @@
       <c r="F293" s="1">
         <v>65624400</v>
       </c>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H293" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F294" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="8" t="s">
         <v>362</v>
       </c>
@@ -6689,13 +7427,13 @@
         <v>510</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B296" s="32"/>
       <c r="F296" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B297" s="30" t="s">
         <v>365</v>
       </c>
@@ -6709,14 +7447,17 @@
       <c r="F297" s="1">
         <v>70710000</v>
       </c>
-    </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H297" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="6"/>
       <c r="F298" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="3"/>
       <c r="B299" s="1" t="s">
         <v>367</v>
@@ -6730,8 +7471,11 @@
       <c r="F299" s="1">
         <v>70711100</v>
       </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H299" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="3"/>
       <c r="B300" s="1" t="s">
         <v>368</v>
@@ -6745,8 +7489,11 @@
       <c r="F300" s="1">
         <v>70711200</v>
       </c>
-    </row>
-    <row r="301" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="H300" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A301" s="3"/>
       <c r="B301" s="1" t="s">
         <v>369</v>
@@ -6760,8 +7507,11 @@
       <c r="F301" s="1">
         <v>70711300</v>
       </c>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H301" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302" s="3"/>
       <c r="B302" s="1" t="s">
         <v>371</v>
@@ -6775,8 +7525,11 @@
       <c r="F302" s="1">
         <v>70711500</v>
       </c>
-    </row>
-    <row r="303" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="H302" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A303" s="3"/>
       <c r="B303" s="1" t="s">
         <v>372</v>
@@ -6790,8 +7543,11 @@
       <c r="F303" s="1">
         <v>70712000</v>
       </c>
-    </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H303" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" s="3"/>
       <c r="B304" s="1" t="s">
         <v>373</v>
@@ -6805,8 +7561,11 @@
       <c r="F304" s="1">
         <v>70713950</v>
       </c>
-    </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H304" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B305" s="1" t="s">
         <v>374</v>
       </c>
@@ -6819,13 +7578,16 @@
       <c r="F305" s="1" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H305" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F306" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B307" s="30" t="s">
         <v>376</v>
       </c>
@@ -6839,14 +7601,17 @@
       <c r="F307" s="1">
         <v>70720000</v>
       </c>
-    </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H307" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="3"/>
       <c r="F308" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="6"/>
       <c r="B309" s="1" t="s">
         <v>378</v>
@@ -6860,8 +7625,11 @@
       <c r="F309" s="1">
         <v>70721100</v>
       </c>
-    </row>
-    <row r="310" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H309" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="3"/>
       <c r="B310" s="1" t="s">
         <v>379</v>
@@ -6878,8 +7646,11 @@
       <c r="G310" s="33" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H310" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311" s="3"/>
       <c r="B311" s="1" t="s">
         <v>381</v>
@@ -6893,8 +7664,11 @@
       <c r="F311" s="1" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H311" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B312" s="1" t="s">
         <v>383</v>
       </c>
@@ -6907,13 +7681,16 @@
       <c r="F312" s="1">
         <v>70722400</v>
       </c>
-    </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H312" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F313" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314" s="8" t="s">
         <v>384</v>
       </c>
@@ -6927,14 +7704,17 @@
       <c r="F314" s="1">
         <v>80000000</v>
       </c>
-    </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H314" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315" s="3"/>
       <c r="F315" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="316" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A316" s="3"/>
       <c r="B316" s="1" t="s">
         <v>386</v>
@@ -6948,8 +7728,11 @@
       <c r="F316" s="1" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H316" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317" s="6"/>
       <c r="B317" s="1" t="s">
         <v>388</v>
@@ -6963,8 +7746,11 @@
       <c r="F317" s="1">
         <v>80811192</v>
       </c>
-    </row>
-    <row r="318" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H317" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A318" s="6"/>
       <c r="B318" s="1" t="s">
         <v>389</v>
@@ -6978,8 +7764,11 @@
       <c r="F318" s="1">
         <v>80811200</v>
       </c>
-    </row>
-    <row r="319" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H318" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A319" s="3"/>
       <c r="B319" s="1" t="s">
         <v>390</v>
@@ -6993,8 +7782,11 @@
       <c r="F319" s="1">
         <v>80811300</v>
       </c>
-    </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H319" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" s="3"/>
       <c r="B320" s="1" t="s">
         <v>391</v>
@@ -7008,8 +7800,11 @@
       <c r="F320" s="1">
         <v>80811400</v>
       </c>
-    </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H320" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" s="3"/>
       <c r="B321" s="1" t="s">
         <v>392</v>
@@ -7026,8 +7821,11 @@
       <c r="G321" s="33" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H321" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" s="3"/>
       <c r="B322" s="1" t="s">
         <v>393</v>
@@ -7044,8 +7842,11 @@
       <c r="G322" s="33" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H322" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" s="3"/>
       <c r="B323" s="1" t="s">
         <v>394</v>
@@ -7059,8 +7860,11 @@
       <c r="F323" s="1" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H323" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" s="3"/>
       <c r="B324" s="1" t="s">
         <v>396</v>
@@ -7074,8 +7878,11 @@
       <c r="F324" s="1">
         <v>80812300</v>
       </c>
-    </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H324" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" s="3"/>
       <c r="B325" s="1" t="s">
         <v>397</v>
@@ -7089,8 +7896,11 @@
       <c r="F325" s="1">
         <v>80812200</v>
       </c>
-    </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H325" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" s="3"/>
       <c r="B326" s="1" t="s">
         <v>398</v>
@@ -7104,8 +7914,11 @@
       <c r="F326" s="1">
         <v>80812900</v>
       </c>
-    </row>
-    <row r="327" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H326" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A327" s="6"/>
       <c r="B327" s="1" t="s">
         <v>399</v>
@@ -7122,8 +7935,11 @@
       <c r="G327" s="33" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="328" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H327" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A328" s="3"/>
       <c r="B328" s="1" t="s">
         <v>400</v>
@@ -7137,8 +7953,11 @@
       <c r="F328" s="1" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H328" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" s="6"/>
       <c r="B329" s="1" t="s">
         <v>402</v>
@@ -7152,8 +7971,11 @@
       <c r="F329" s="1">
         <v>80813930</v>
       </c>
-    </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H329" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" s="3"/>
       <c r="B330" s="1" t="s">
         <v>403</v>
@@ -7167,8 +7989,11 @@
       <c r="F330" s="1" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="331" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H330" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B331" s="1" t="s">
         <v>405</v>
       </c>
@@ -7184,13 +8009,16 @@
       <c r="G331" s="33" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H331" s="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F332" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" s="8" t="s">
         <v>406</v>
       </c>
@@ -7206,14 +8034,17 @@
       <c r="G333" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H333" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" s="3"/>
       <c r="F334" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="335" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A335" s="3"/>
       <c r="B335" s="1" t="s">
         <v>408</v>
@@ -7230,8 +8061,11 @@
       <c r="G335" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H335" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" s="3"/>
       <c r="B336" s="1" t="s">
         <v>410</v>
@@ -7248,8 +8082,11 @@
       <c r="G336" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H336" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="3"/>
       <c r="B337" s="1" t="s">
         <v>411</v>
@@ -7266,8 +8103,11 @@
       <c r="G337" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H337" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="3"/>
       <c r="B338" s="1" t="s">
         <v>412</v>
@@ -7284,8 +8124,11 @@
       <c r="G338" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H338" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="6"/>
       <c r="B339" s="1" t="s">
         <v>414</v>
@@ -7302,8 +8145,11 @@
       <c r="G339" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="340" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H339" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="340" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A340" s="6"/>
       <c r="B340" s="1" t="s">
         <v>415</v>
@@ -7320,8 +8166,11 @@
       <c r="G340" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H340" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" s="3"/>
       <c r="B341" s="1" t="s">
         <v>417</v>
@@ -7338,8 +8187,11 @@
       <c r="G341" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H341" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B342" s="1" t="s">
         <v>419</v>
       </c>
@@ -7355,13 +8207,19 @@
       <c r="G342" s="33" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H342" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F343" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H343" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344" s="8" t="s">
         <v>420</v>
       </c>
@@ -7377,15 +8235,21 @@
       <c r="G344" s="33" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H344" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B345" s="20"/>
       <c r="D345" s="3"/>
       <c r="F345" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H345" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" s="3"/>
       <c r="B346" s="1" t="s">
         <v>422</v>
@@ -7402,8 +8266,11 @@
       <c r="G346" s="33" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H346" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" s="3"/>
       <c r="B347" s="1" t="s">
         <v>423</v>
@@ -7420,8 +8287,11 @@
       <c r="G347" s="33" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H347" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" s="3"/>
       <c r="B348" s="1" t="s">
         <v>424</v>
@@ -7438,8 +8308,11 @@
       <c r="G348" s="33" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H348" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" s="3"/>
       <c r="B349" s="1" t="s">
         <v>425</v>
@@ -7456,8 +8329,11 @@
       <c r="G349" s="33" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H349" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B350" s="1" t="s">
         <v>426</v>
       </c>
@@ -7473,8 +8349,11 @@
       <c r="G350" s="33" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H350" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B351" s="1" t="s">
         <v>427</v>
       </c>
@@ -7490,8 +8369,11 @@
       <c r="G351" s="33" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H351" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B352" s="1" t="s">
         <v>428</v>
       </c>
@@ -7506,6 +8388,9 @@
       </c>
       <c r="G352" s="33" t="s">
         <v>525</v>
+      </c>
+      <c r="H352" s="1">
+        <v>92</v>
       </c>
     </row>
     <row r="353" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Small note on private households likely not included in CES
</commit_message>
<xml_diff>
--- a/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
+++ b/data/manual-files/2017-industry-code-list-ces-crosswalk-manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\GMacDonald\Documents\ipums-acs-naics-standardization\data\manual-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A748D6F6-4234-4FC2-A47F-4DBFDD4BF466}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D68E0B7-6A99-4BDB-AF11-D235B5AA9717}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1611,9 +1611,6 @@
     <t>Made a decision to calculate it as the residual of 813</t>
   </si>
   <si>
-    <t>Made a decision to calculate as the residual of 81</t>
-  </si>
-  <si>
     <t>Made a decision to code as general government, no subcodes available, minus military and postal service</t>
   </si>
   <si>
@@ -1678,6 +1675,9 @@
   </si>
   <si>
     <t>Made decision to treat residuals as category minus everything else defined, could be 0, given other definitions and decisions made here, for 2 digit NAICS made arbitrary decision to assign to 44</t>
+  </si>
+  <si>
+    <t>Made a decision to calculate as the residual of 81, BLS likely does not include given this is an establishment survey, can likely assume 0 change</t>
   </si>
 </sst>
 </file>
@@ -2148,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+      <selection activeCell="G331" sqref="G331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,7 +2195,7 @@
         <v>437</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2229,10 +2229,10 @@
         <v>6</v>
       </c>
       <c r="F7" s="33" t="s">
+        <v>526</v>
+      </c>
+      <c r="G7" s="33" t="s">
         <v>527</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2470,10 +2470,10 @@
         <v>34</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="G24" s="33" t="s">
         <v>529</v>
-      </c>
-      <c r="G24" s="33" t="s">
-        <v>530</v>
       </c>
       <c r="H24" s="1">
         <v>21</v>
@@ -2704,10 +2704,10 @@
         <v>55</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H41" s="1">
         <v>31</v>
@@ -2911,10 +2911,10 @@
         <v>3162</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H51" s="1">
         <v>31</v>
@@ -2932,10 +2932,10 @@
         <v>71</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H52" s="1">
         <v>31</v>
@@ -3560,10 +3560,10 @@
         <v>113</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G84" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H84" s="1">
         <v>33</v>
@@ -3700,10 +3700,10 @@
         <v>121</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G90" s="33" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H90" s="1">
         <v>33</v>
@@ -4181,10 +4181,10 @@
         <v>152</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G111" s="33" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H111" s="1">
         <v>33</v>
@@ -4611,10 +4611,10 @@
         <v>179</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G135" s="33" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H135" s="1">
         <v>42</v>
@@ -5323,10 +5323,10 @@
         <v>220</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G173" s="33" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H173" s="1">
         <v>44</v>
@@ -5778,10 +5778,10 @@
         <v>256</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G199" s="33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H199" s="1">
         <v>22</v>
@@ -7330,7 +7330,7 @@
         <v>357</v>
       </c>
       <c r="F289" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="H289" s="1">
         <v>62</v>
@@ -8004,10 +8004,10 @@
         <v>814</v>
       </c>
       <c r="F331" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G331" s="33" t="s">
-        <v>522</v>
+        <v>544</v>
       </c>
       <c r="H331" s="1">
         <v>81</v>
@@ -8029,10 +8029,10 @@
         <v>92</v>
       </c>
       <c r="F333" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G333" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H333" s="1">
         <v>92</v>
@@ -8056,10 +8056,10 @@
         <v>409</v>
       </c>
       <c r="F335" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G335" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H335" s="1">
         <v>92</v>
@@ -8077,10 +8077,10 @@
         <v>92113</v>
       </c>
       <c r="F336" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G336" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H336" s="1">
         <v>92</v>
@@ -8098,10 +8098,10 @@
         <v>92119</v>
       </c>
       <c r="F337" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G337" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H337" s="1">
         <v>92</v>
@@ -8119,10 +8119,10 @@
         <v>413</v>
       </c>
       <c r="F338" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G338" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H338" s="1">
         <v>92</v>
@@ -8140,10 +8140,10 @@
         <v>923</v>
       </c>
       <c r="F339" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G339" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H339" s="1">
         <v>92</v>
@@ -8161,10 +8161,10 @@
         <v>416</v>
       </c>
       <c r="F340" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G340" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H340" s="1">
         <v>92</v>
@@ -8182,10 +8182,10 @@
         <v>418</v>
       </c>
       <c r="F341" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G341" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H341" s="1">
         <v>92</v>
@@ -8202,10 +8202,10 @@
         <v>928</v>
       </c>
       <c r="F342" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G342" s="33" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H342" s="1">
         <v>92</v>
@@ -8233,7 +8233,7 @@
         <v>90919110</v>
       </c>
       <c r="G344" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H344" s="1">
         <v>92</v>
@@ -8264,7 +8264,7 @@
         <v>90919110</v>
       </c>
       <c r="G346" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H346" s="1">
         <v>92</v>
@@ -8285,7 +8285,7 @@
         <v>90919110</v>
       </c>
       <c r="G347" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H347" s="1">
         <v>92</v>
@@ -8306,7 +8306,7 @@
         <v>90919110</v>
       </c>
       <c r="G348" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H348" s="1">
         <v>92</v>
@@ -8327,7 +8327,7 @@
         <v>90919110</v>
       </c>
       <c r="G349" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H349" s="1">
         <v>92</v>
@@ -8347,7 +8347,7 @@
         <v>90919110</v>
       </c>
       <c r="G350" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H350" s="1">
         <v>92</v>
@@ -8367,7 +8367,7 @@
         <v>90919110</v>
       </c>
       <c r="G351" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H351" s="1">
         <v>92</v>
@@ -8387,7 +8387,7 @@
         <v>90919110</v>
       </c>
       <c r="G352" s="33" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H352" s="1">
         <v>92</v>

</xml_diff>